<commit_message>
Revised Template Finish Fet Plan sheet
</commit_message>
<xml_diff>
--- a/wizard/FinishFetplan.xlsx
+++ b/wizard/FinishFetplan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="29">
   <si>
     <t>Colour coding for Job In Finish Fettling F2</t>
   </si>
@@ -696,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -840,42 +840,12 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -889,6 +859,37 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6098,7 +6099,7 @@
       <pane xSplit="3" ySplit="24" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
-      <selection pane="bottomRight" sqref="A1:B1"/>
+      <selection pane="bottomRight" activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6110,10 +6111,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:291" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="72"/>
+      <c r="A1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="80"/>
       <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
@@ -6124,15 +6125,9 @@
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
       <c r="J1" s="21"/>
-      <c r="K1" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>4</v>
-      </c>
+      <c r="K1" s="22"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
       <c r="N1" s="23"/>
     </row>
     <row r="2" spans="1:291" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -6141,24 +6136,18 @@
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="7">
-        <v>8</v>
-      </c>
-      <c r="L2" s="7">
-        <v>16</v>
-      </c>
-      <c r="M2" s="7">
-        <v>16</v>
-      </c>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
       <c r="N2" s="25"/>
     </row>
     <row r="3" spans="1:291" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6171,24 +6160,18 @@
       <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="81" t="s">
+      <c r="D3" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="7">
-        <v>9</v>
-      </c>
-      <c r="L3" s="7">
-        <v>9</v>
-      </c>
-      <c r="M3" s="7">
-        <v>9</v>
-      </c>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
       <c r="N3" s="25"/>
     </row>
     <row r="4" spans="1:291" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -6197,24 +6180,18 @@
       <c r="C4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="7">
-        <v>1</v>
-      </c>
-      <c r="L4" s="7">
-        <v>2</v>
-      </c>
-      <c r="M4" s="7">
-        <v>2</v>
-      </c>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
       <c r="N4" s="25"/>
     </row>
     <row r="5" spans="1:291" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -6227,15 +6204,15 @@
       <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="83">
+      <c r="D5" s="88">
         <v>627</v>
       </c>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="84"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="89"/>
       <c r="K5" s="19"/>
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
@@ -6315,298 +6292,298 @@
     </row>
     <row r="10" spans="1:291" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:291" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="89" t="s">
+      <c r="B11" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="90"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="73"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="72"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="71"/>
-      <c r="N11" s="72"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="71"/>
-      <c r="Q11" s="72"/>
-      <c r="R11" s="73"/>
-      <c r="S11" s="71"/>
-      <c r="T11" s="72"/>
-      <c r="U11" s="73"/>
-      <c r="V11" s="71"/>
-      <c r="W11" s="72"/>
-      <c r="X11" s="73"/>
-      <c r="Y11" s="71"/>
-      <c r="Z11" s="72"/>
-      <c r="AA11" s="73"/>
-      <c r="AB11" s="71"/>
-      <c r="AC11" s="72"/>
-      <c r="AD11" s="73"/>
-      <c r="AE11" s="71"/>
-      <c r="AF11" s="72"/>
-      <c r="AG11" s="73"/>
-      <c r="AH11" s="71"/>
-      <c r="AI11" s="72"/>
-      <c r="AJ11" s="73"/>
-      <c r="AK11" s="71"/>
-      <c r="AL11" s="72"/>
-      <c r="AM11" s="73"/>
-      <c r="AN11" s="71"/>
-      <c r="AO11" s="72"/>
-      <c r="AP11" s="73"/>
-      <c r="AQ11" s="71"/>
-      <c r="AR11" s="72"/>
-      <c r="AS11" s="73"/>
-      <c r="AT11" s="71"/>
-      <c r="AU11" s="72"/>
-      <c r="AV11" s="73"/>
-      <c r="AW11" s="71"/>
-      <c r="AX11" s="72"/>
-      <c r="AY11" s="73"/>
-      <c r="AZ11" s="71"/>
-      <c r="BA11" s="72"/>
-      <c r="BB11" s="73"/>
-      <c r="BC11" s="71"/>
-      <c r="BD11" s="72"/>
-      <c r="BE11" s="73"/>
-      <c r="BF11" s="71"/>
-      <c r="BG11" s="72"/>
-      <c r="BH11" s="73"/>
-      <c r="BI11" s="71"/>
-      <c r="BJ11" s="72"/>
-      <c r="BK11" s="73"/>
-      <c r="BL11" s="71"/>
-      <c r="BM11" s="72"/>
-      <c r="BN11" s="73"/>
-      <c r="BO11" s="71"/>
-      <c r="BP11" s="72"/>
-      <c r="BQ11" s="73"/>
-      <c r="BR11" s="71"/>
-      <c r="BS11" s="72"/>
-      <c r="BT11" s="73"/>
-      <c r="BU11" s="71"/>
-      <c r="BV11" s="72"/>
-      <c r="BW11" s="73"/>
-      <c r="BX11" s="71"/>
-      <c r="BY11" s="72"/>
-      <c r="BZ11" s="73"/>
-      <c r="CA11" s="71"/>
-      <c r="CB11" s="72"/>
-      <c r="CC11" s="73"/>
-      <c r="CD11" s="71"/>
-      <c r="CE11" s="72"/>
-      <c r="CF11" s="73"/>
-      <c r="CG11" s="71"/>
-      <c r="CH11" s="72"/>
-      <c r="CI11" s="73"/>
-      <c r="CJ11" s="71"/>
-      <c r="CK11" s="72"/>
-      <c r="CL11" s="73"/>
-      <c r="CM11" s="71"/>
-      <c r="CN11" s="72"/>
-      <c r="CO11" s="73"/>
-      <c r="CP11" s="71"/>
-      <c r="CQ11" s="72"/>
-      <c r="CR11" s="73"/>
-      <c r="CS11" s="71"/>
-      <c r="CT11" s="72"/>
-      <c r="CU11" s="73"/>
-      <c r="CV11" s="71"/>
-      <c r="CW11" s="72"/>
-      <c r="CX11" s="73"/>
-      <c r="CY11" s="71"/>
-      <c r="CZ11" s="72"/>
-      <c r="DA11" s="73"/>
-      <c r="DB11" s="71"/>
-      <c r="DC11" s="72"/>
-      <c r="DD11" s="73"/>
-      <c r="DE11" s="71"/>
-      <c r="DF11" s="72"/>
-      <c r="DG11" s="73"/>
-      <c r="DH11" s="71"/>
-      <c r="DI11" s="72"/>
-      <c r="DJ11" s="73"/>
-      <c r="DK11" s="71"/>
-      <c r="DL11" s="72"/>
-      <c r="DM11" s="73"/>
-      <c r="DN11" s="71"/>
-      <c r="DO11" s="72"/>
-      <c r="DP11" s="73"/>
-      <c r="DQ11" s="71"/>
-      <c r="DR11" s="72"/>
-      <c r="DS11" s="73"/>
-      <c r="DT11" s="71"/>
-      <c r="DU11" s="72"/>
-      <c r="DV11" s="73"/>
-      <c r="DW11" s="71"/>
-      <c r="DX11" s="72"/>
-      <c r="DY11" s="73"/>
-      <c r="DZ11" s="71"/>
-      <c r="EA11" s="72"/>
-      <c r="EB11" s="73"/>
-      <c r="EC11" s="71"/>
-      <c r="ED11" s="72"/>
-      <c r="EE11" s="73"/>
-      <c r="EF11" s="71"/>
-      <c r="EG11" s="72"/>
-      <c r="EH11" s="73"/>
-      <c r="EI11" s="71"/>
-      <c r="EJ11" s="72"/>
-      <c r="EK11" s="73"/>
-      <c r="EL11" s="71"/>
-      <c r="EM11" s="72"/>
-      <c r="EN11" s="73"/>
-      <c r="EO11" s="71"/>
-      <c r="EP11" s="72"/>
-      <c r="EQ11" s="73"/>
-      <c r="ER11" s="71"/>
-      <c r="ES11" s="72"/>
-      <c r="ET11" s="73"/>
-      <c r="EU11" s="71"/>
-      <c r="EV11" s="72"/>
-      <c r="EW11" s="73"/>
-      <c r="EX11" s="71"/>
-      <c r="EY11" s="72"/>
-      <c r="EZ11" s="73"/>
-      <c r="FA11" s="71"/>
-      <c r="FB11" s="72"/>
-      <c r="FC11" s="73"/>
-      <c r="FD11" s="71"/>
-      <c r="FE11" s="72"/>
-      <c r="FF11" s="73"/>
-      <c r="FG11" s="71"/>
-      <c r="FH11" s="72"/>
-      <c r="FI11" s="73"/>
-      <c r="FJ11" s="71"/>
-      <c r="FK11" s="72"/>
-      <c r="FL11" s="73"/>
-      <c r="FM11" s="71"/>
-      <c r="FN11" s="72"/>
-      <c r="FO11" s="73"/>
-      <c r="FP11" s="71"/>
-      <c r="FQ11" s="72"/>
-      <c r="FR11" s="73"/>
-      <c r="FS11" s="71"/>
-      <c r="FT11" s="72"/>
-      <c r="FU11" s="73"/>
-      <c r="FV11" s="71"/>
-      <c r="FW11" s="72"/>
-      <c r="FX11" s="73"/>
-      <c r="FY11" s="71"/>
-      <c r="FZ11" s="72"/>
-      <c r="GA11" s="73"/>
-      <c r="GB11" s="71"/>
-      <c r="GC11" s="72"/>
-      <c r="GD11" s="73"/>
-      <c r="GE11" s="71"/>
-      <c r="GF11" s="72"/>
-      <c r="GG11" s="73"/>
-      <c r="GH11" s="71"/>
-      <c r="GI11" s="72"/>
-      <c r="GJ11" s="73"/>
-      <c r="GK11" s="71"/>
-      <c r="GL11" s="72"/>
-      <c r="GM11" s="73"/>
-      <c r="GN11" s="71"/>
-      <c r="GO11" s="72"/>
-      <c r="GP11" s="73"/>
-      <c r="GQ11" s="71"/>
-      <c r="GR11" s="72"/>
-      <c r="GS11" s="73"/>
-      <c r="GT11" s="71"/>
-      <c r="GU11" s="72"/>
-      <c r="GV11" s="73"/>
-      <c r="GW11" s="71"/>
-      <c r="GX11" s="72"/>
-      <c r="GY11" s="73"/>
-      <c r="GZ11" s="71"/>
-      <c r="HA11" s="72"/>
-      <c r="HB11" s="73"/>
-      <c r="HC11" s="71"/>
-      <c r="HD11" s="72"/>
-      <c r="HE11" s="73"/>
-      <c r="HF11" s="71"/>
-      <c r="HG11" s="72"/>
-      <c r="HH11" s="73"/>
-      <c r="HI11" s="71"/>
-      <c r="HJ11" s="72"/>
-      <c r="HK11" s="73"/>
-      <c r="HL11" s="71"/>
-      <c r="HM11" s="72"/>
-      <c r="HN11" s="73"/>
-      <c r="HO11" s="71"/>
-      <c r="HP11" s="72"/>
-      <c r="HQ11" s="73"/>
-      <c r="HR11" s="71"/>
-      <c r="HS11" s="72"/>
-      <c r="HT11" s="73"/>
-      <c r="HU11" s="71"/>
-      <c r="HV11" s="72"/>
-      <c r="HW11" s="73"/>
-      <c r="HX11" s="71"/>
-      <c r="HY11" s="72"/>
-      <c r="HZ11" s="73"/>
-      <c r="IA11" s="71"/>
-      <c r="IB11" s="72"/>
-      <c r="IC11" s="73"/>
-      <c r="ID11" s="71"/>
-      <c r="IE11" s="72"/>
-      <c r="IF11" s="73"/>
-      <c r="IG11" s="71"/>
-      <c r="IH11" s="72"/>
-      <c r="II11" s="73"/>
-      <c r="IJ11" s="71"/>
-      <c r="IK11" s="72"/>
-      <c r="IL11" s="73"/>
-      <c r="IM11" s="71"/>
-      <c r="IN11" s="72"/>
-      <c r="IO11" s="73"/>
-      <c r="IP11" s="71"/>
-      <c r="IQ11" s="72"/>
-      <c r="IR11" s="73"/>
-      <c r="IS11" s="71"/>
-      <c r="IT11" s="72"/>
-      <c r="IU11" s="73"/>
-      <c r="IV11" s="71"/>
-      <c r="IW11" s="72"/>
-      <c r="IX11" s="73"/>
-      <c r="IY11" s="71"/>
-      <c r="IZ11" s="72"/>
-      <c r="JA11" s="73"/>
-      <c r="JB11" s="71"/>
-      <c r="JC11" s="72"/>
-      <c r="JD11" s="73"/>
-      <c r="JE11" s="71"/>
-      <c r="JF11" s="72"/>
-      <c r="JG11" s="73"/>
-      <c r="JH11" s="71"/>
-      <c r="JI11" s="72"/>
-      <c r="JJ11" s="73"/>
-      <c r="JK11" s="71"/>
-      <c r="JL11" s="72"/>
-      <c r="JM11" s="73"/>
-      <c r="JN11" s="71"/>
-      <c r="JO11" s="72"/>
-      <c r="JP11" s="73"/>
-      <c r="JQ11" s="71"/>
-      <c r="JR11" s="72"/>
-      <c r="JS11" s="73"/>
-      <c r="JT11" s="71"/>
-      <c r="JU11" s="72"/>
-      <c r="JV11" s="73"/>
-      <c r="JW11" s="71"/>
-      <c r="JX11" s="72"/>
-      <c r="JY11" s="73"/>
-      <c r="JZ11" s="71"/>
-      <c r="KA11" s="72"/>
-      <c r="KB11" s="73"/>
-      <c r="KC11" s="71"/>
-      <c r="KD11" s="72"/>
-      <c r="KE11" s="73"/>
+      <c r="C11" s="76"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="80"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="79"/>
+      <c r="N11" s="80"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="79"/>
+      <c r="Q11" s="80"/>
+      <c r="R11" s="81"/>
+      <c r="S11" s="79"/>
+      <c r="T11" s="80"/>
+      <c r="U11" s="81"/>
+      <c r="V11" s="79"/>
+      <c r="W11" s="80"/>
+      <c r="X11" s="81"/>
+      <c r="Y11" s="79"/>
+      <c r="Z11" s="80"/>
+      <c r="AA11" s="81"/>
+      <c r="AB11" s="79"/>
+      <c r="AC11" s="80"/>
+      <c r="AD11" s="81"/>
+      <c r="AE11" s="79"/>
+      <c r="AF11" s="80"/>
+      <c r="AG11" s="81"/>
+      <c r="AH11" s="79"/>
+      <c r="AI11" s="80"/>
+      <c r="AJ11" s="81"/>
+      <c r="AK11" s="79"/>
+      <c r="AL11" s="80"/>
+      <c r="AM11" s="81"/>
+      <c r="AN11" s="79"/>
+      <c r="AO11" s="80"/>
+      <c r="AP11" s="81"/>
+      <c r="AQ11" s="79"/>
+      <c r="AR11" s="80"/>
+      <c r="AS11" s="81"/>
+      <c r="AT11" s="79"/>
+      <c r="AU11" s="80"/>
+      <c r="AV11" s="81"/>
+      <c r="AW11" s="79"/>
+      <c r="AX11" s="80"/>
+      <c r="AY11" s="81"/>
+      <c r="AZ11" s="79"/>
+      <c r="BA11" s="80"/>
+      <c r="BB11" s="81"/>
+      <c r="BC11" s="79"/>
+      <c r="BD11" s="80"/>
+      <c r="BE11" s="81"/>
+      <c r="BF11" s="79"/>
+      <c r="BG11" s="80"/>
+      <c r="BH11" s="81"/>
+      <c r="BI11" s="79"/>
+      <c r="BJ11" s="80"/>
+      <c r="BK11" s="81"/>
+      <c r="BL11" s="79"/>
+      <c r="BM11" s="80"/>
+      <c r="BN11" s="81"/>
+      <c r="BO11" s="79"/>
+      <c r="BP11" s="80"/>
+      <c r="BQ11" s="81"/>
+      <c r="BR11" s="79"/>
+      <c r="BS11" s="80"/>
+      <c r="BT11" s="81"/>
+      <c r="BU11" s="79"/>
+      <c r="BV11" s="80"/>
+      <c r="BW11" s="81"/>
+      <c r="BX11" s="79"/>
+      <c r="BY11" s="80"/>
+      <c r="BZ11" s="81"/>
+      <c r="CA11" s="79"/>
+      <c r="CB11" s="80"/>
+      <c r="CC11" s="81"/>
+      <c r="CD11" s="79"/>
+      <c r="CE11" s="80"/>
+      <c r="CF11" s="81"/>
+      <c r="CG11" s="79"/>
+      <c r="CH11" s="80"/>
+      <c r="CI11" s="81"/>
+      <c r="CJ11" s="79"/>
+      <c r="CK11" s="80"/>
+      <c r="CL11" s="81"/>
+      <c r="CM11" s="79"/>
+      <c r="CN11" s="80"/>
+      <c r="CO11" s="81"/>
+      <c r="CP11" s="79"/>
+      <c r="CQ11" s="80"/>
+      <c r="CR11" s="81"/>
+      <c r="CS11" s="79"/>
+      <c r="CT11" s="80"/>
+      <c r="CU11" s="81"/>
+      <c r="CV11" s="79"/>
+      <c r="CW11" s="80"/>
+      <c r="CX11" s="81"/>
+      <c r="CY11" s="79"/>
+      <c r="CZ11" s="80"/>
+      <c r="DA11" s="81"/>
+      <c r="DB11" s="79"/>
+      <c r="DC11" s="80"/>
+      <c r="DD11" s="81"/>
+      <c r="DE11" s="79"/>
+      <c r="DF11" s="80"/>
+      <c r="DG11" s="81"/>
+      <c r="DH11" s="79"/>
+      <c r="DI11" s="80"/>
+      <c r="DJ11" s="81"/>
+      <c r="DK11" s="79"/>
+      <c r="DL11" s="80"/>
+      <c r="DM11" s="81"/>
+      <c r="DN11" s="79"/>
+      <c r="DO11" s="80"/>
+      <c r="DP11" s="81"/>
+      <c r="DQ11" s="79"/>
+      <c r="DR11" s="80"/>
+      <c r="DS11" s="81"/>
+      <c r="DT11" s="79"/>
+      <c r="DU11" s="80"/>
+      <c r="DV11" s="81"/>
+      <c r="DW11" s="79"/>
+      <c r="DX11" s="80"/>
+      <c r="DY11" s="81"/>
+      <c r="DZ11" s="79"/>
+      <c r="EA11" s="80"/>
+      <c r="EB11" s="81"/>
+      <c r="EC11" s="79"/>
+      <c r="ED11" s="80"/>
+      <c r="EE11" s="81"/>
+      <c r="EF11" s="79"/>
+      <c r="EG11" s="80"/>
+      <c r="EH11" s="81"/>
+      <c r="EI11" s="79"/>
+      <c r="EJ11" s="80"/>
+      <c r="EK11" s="81"/>
+      <c r="EL11" s="79"/>
+      <c r="EM11" s="80"/>
+      <c r="EN11" s="81"/>
+      <c r="EO11" s="79"/>
+      <c r="EP11" s="80"/>
+      <c r="EQ11" s="81"/>
+      <c r="ER11" s="79"/>
+      <c r="ES11" s="80"/>
+      <c r="ET11" s="81"/>
+      <c r="EU11" s="79"/>
+      <c r="EV11" s="80"/>
+      <c r="EW11" s="81"/>
+      <c r="EX11" s="79"/>
+      <c r="EY11" s="80"/>
+      <c r="EZ11" s="81"/>
+      <c r="FA11" s="79"/>
+      <c r="FB11" s="80"/>
+      <c r="FC11" s="81"/>
+      <c r="FD11" s="79"/>
+      <c r="FE11" s="80"/>
+      <c r="FF11" s="81"/>
+      <c r="FG11" s="79"/>
+      <c r="FH11" s="80"/>
+      <c r="FI11" s="81"/>
+      <c r="FJ11" s="79"/>
+      <c r="FK11" s="80"/>
+      <c r="FL11" s="81"/>
+      <c r="FM11" s="79"/>
+      <c r="FN11" s="80"/>
+      <c r="FO11" s="81"/>
+      <c r="FP11" s="79"/>
+      <c r="FQ11" s="80"/>
+      <c r="FR11" s="81"/>
+      <c r="FS11" s="79"/>
+      <c r="FT11" s="80"/>
+      <c r="FU11" s="81"/>
+      <c r="FV11" s="79"/>
+      <c r="FW11" s="80"/>
+      <c r="FX11" s="81"/>
+      <c r="FY11" s="79"/>
+      <c r="FZ11" s="80"/>
+      <c r="GA11" s="81"/>
+      <c r="GB11" s="79"/>
+      <c r="GC11" s="80"/>
+      <c r="GD11" s="81"/>
+      <c r="GE11" s="79"/>
+      <c r="GF11" s="80"/>
+      <c r="GG11" s="81"/>
+      <c r="GH11" s="79"/>
+      <c r="GI11" s="80"/>
+      <c r="GJ11" s="81"/>
+      <c r="GK11" s="79"/>
+      <c r="GL11" s="80"/>
+      <c r="GM11" s="81"/>
+      <c r="GN11" s="79"/>
+      <c r="GO11" s="80"/>
+      <c r="GP11" s="81"/>
+      <c r="GQ11" s="79"/>
+      <c r="GR11" s="80"/>
+      <c r="GS11" s="81"/>
+      <c r="GT11" s="79"/>
+      <c r="GU11" s="80"/>
+      <c r="GV11" s="81"/>
+      <c r="GW11" s="79"/>
+      <c r="GX11" s="80"/>
+      <c r="GY11" s="81"/>
+      <c r="GZ11" s="79"/>
+      <c r="HA11" s="80"/>
+      <c r="HB11" s="81"/>
+      <c r="HC11" s="79"/>
+      <c r="HD11" s="80"/>
+      <c r="HE11" s="81"/>
+      <c r="HF11" s="79"/>
+      <c r="HG11" s="80"/>
+      <c r="HH11" s="81"/>
+      <c r="HI11" s="79"/>
+      <c r="HJ11" s="80"/>
+      <c r="HK11" s="81"/>
+      <c r="HL11" s="79"/>
+      <c r="HM11" s="80"/>
+      <c r="HN11" s="81"/>
+      <c r="HO11" s="79"/>
+      <c r="HP11" s="80"/>
+      <c r="HQ11" s="81"/>
+      <c r="HR11" s="79"/>
+      <c r="HS11" s="80"/>
+      <c r="HT11" s="81"/>
+      <c r="HU11" s="79"/>
+      <c r="HV11" s="80"/>
+      <c r="HW11" s="81"/>
+      <c r="HX11" s="79"/>
+      <c r="HY11" s="80"/>
+      <c r="HZ11" s="81"/>
+      <c r="IA11" s="79"/>
+      <c r="IB11" s="80"/>
+      <c r="IC11" s="81"/>
+      <c r="ID11" s="79"/>
+      <c r="IE11" s="80"/>
+      <c r="IF11" s="81"/>
+      <c r="IG11" s="79"/>
+      <c r="IH11" s="80"/>
+      <c r="II11" s="81"/>
+      <c r="IJ11" s="79"/>
+      <c r="IK11" s="80"/>
+      <c r="IL11" s="81"/>
+      <c r="IM11" s="79"/>
+      <c r="IN11" s="80"/>
+      <c r="IO11" s="81"/>
+      <c r="IP11" s="79"/>
+      <c r="IQ11" s="80"/>
+      <c r="IR11" s="81"/>
+      <c r="IS11" s="79"/>
+      <c r="IT11" s="80"/>
+      <c r="IU11" s="81"/>
+      <c r="IV11" s="79"/>
+      <c r="IW11" s="80"/>
+      <c r="IX11" s="81"/>
+      <c r="IY11" s="79"/>
+      <c r="IZ11" s="80"/>
+      <c r="JA11" s="81"/>
+      <c r="JB11" s="79"/>
+      <c r="JC11" s="80"/>
+      <c r="JD11" s="81"/>
+      <c r="JE11" s="79"/>
+      <c r="JF11" s="80"/>
+      <c r="JG11" s="81"/>
+      <c r="JH11" s="79"/>
+      <c r="JI11" s="80"/>
+      <c r="JJ11" s="81"/>
+      <c r="JK11" s="79"/>
+      <c r="JL11" s="80"/>
+      <c r="JM11" s="81"/>
+      <c r="JN11" s="79"/>
+      <c r="JO11" s="80"/>
+      <c r="JP11" s="81"/>
+      <c r="JQ11" s="79"/>
+      <c r="JR11" s="80"/>
+      <c r="JS11" s="81"/>
+      <c r="JT11" s="79"/>
+      <c r="JU11" s="80"/>
+      <c r="JV11" s="81"/>
+      <c r="JW11" s="79"/>
+      <c r="JX11" s="80"/>
+      <c r="JY11" s="81"/>
+      <c r="JZ11" s="79"/>
+      <c r="KA11" s="80"/>
+      <c r="KB11" s="81"/>
+      <c r="KC11" s="79"/>
+      <c r="KD11" s="80"/>
+      <c r="KE11" s="81"/>
     </row>
     <row r="12" spans="1:291" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="36"/>
@@ -7477,7 +7454,7 @@
       </c>
     </row>
     <row r="13" spans="1:291" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="82" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="40" t="s">
@@ -7773,7 +7750,7 @@
       <c r="KE13" s="46"/>
     </row>
     <row r="14" spans="1:291" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="86"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="41" t="s">
         <v>26</v>
       </c>
@@ -9094,7 +9071,7 @@
         <v>0</v>
       </c>
       <c r="IZ15" s="69">
-        <f t="shared" ref="IZ15:LK15" si="4">IZ13-IZ14</f>
+        <f t="shared" ref="IZ15:KE15" si="4">IZ13-IZ14</f>
         <v>0</v>
       </c>
       <c r="JA15" s="70">
@@ -9224,7 +9201,7 @@
     </row>
     <row r="16" spans="1:291" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
-      <c r="B16" s="88" t="s">
+      <c r="B16" s="84" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="42" t="s">
@@ -9520,7 +9497,7 @@
       <c r="KE16" s="46"/>
     </row>
     <row r="17" spans="1:291" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="86"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="41" t="s">
         <v>26</v>
       </c>
@@ -10970,7 +10947,7 @@
       </c>
     </row>
     <row r="19" spans="1:291" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="85" t="s">
+      <c r="B19" s="93" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="42" t="s">
@@ -11266,7 +11243,7 @@
       <c r="KE19" s="46"/>
     </row>
     <row r="20" spans="1:291" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="86"/>
+      <c r="B20" s="83"/>
       <c r="C20" s="41" t="s">
         <v>26</v>
       </c>
@@ -12905,10 +12882,10 @@
     </row>
     <row r="23" spans="1:291" x14ac:dyDescent="0.25">
       <c r="A23" s="63"/>
-      <c r="B23" s="91" t="s">
+      <c r="B23" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="92"/>
+      <c r="C23" s="78"/>
       <c r="D23" s="51"/>
       <c r="E23" s="6"/>
       <c r="F23" s="52"/>
@@ -13106,192 +13083,192 @@
       <c r="C24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="77"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="77"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="79"/>
-      <c r="J24" s="77"/>
-      <c r="K24" s="78"/>
-      <c r="L24" s="79"/>
-      <c r="M24" s="77"/>
-      <c r="N24" s="78"/>
-      <c r="O24" s="79"/>
-      <c r="P24" s="77"/>
-      <c r="Q24" s="78"/>
-      <c r="R24" s="79"/>
-      <c r="S24" s="77"/>
-      <c r="T24" s="78"/>
-      <c r="U24" s="79"/>
-      <c r="V24" s="77"/>
-      <c r="W24" s="78"/>
-      <c r="X24" s="79"/>
-      <c r="Y24" s="77"/>
-      <c r="Z24" s="78"/>
-      <c r="AA24" s="79"/>
-      <c r="AB24" s="77"/>
-      <c r="AC24" s="78"/>
-      <c r="AD24" s="79"/>
-      <c r="AE24" s="77"/>
-      <c r="AF24" s="78"/>
-      <c r="AG24" s="79"/>
-      <c r="AH24" s="77"/>
-      <c r="AI24" s="78"/>
-      <c r="AJ24" s="79"/>
-      <c r="AK24" s="77"/>
-      <c r="AL24" s="78"/>
-      <c r="AM24" s="79"/>
-      <c r="AN24" s="77"/>
-      <c r="AO24" s="78"/>
-      <c r="AP24" s="79"/>
-      <c r="AQ24" s="77"/>
-      <c r="AR24" s="78"/>
-      <c r="AS24" s="79"/>
-      <c r="AT24" s="77"/>
-      <c r="AU24" s="78"/>
-      <c r="AV24" s="79"/>
-      <c r="AW24" s="77"/>
-      <c r="AX24" s="78"/>
-      <c r="AY24" s="79"/>
-      <c r="AZ24" s="77"/>
-      <c r="BA24" s="78"/>
-      <c r="BB24" s="79"/>
-      <c r="BC24" s="77"/>
-      <c r="BD24" s="78"/>
-      <c r="BE24" s="79"/>
-      <c r="BF24" s="77"/>
-      <c r="BG24" s="78"/>
-      <c r="BH24" s="79"/>
-      <c r="BI24" s="77"/>
-      <c r="BJ24" s="78"/>
-      <c r="BK24" s="79"/>
-      <c r="BL24" s="77"/>
-      <c r="BM24" s="78"/>
-      <c r="BN24" s="79"/>
-      <c r="BO24" s="77"/>
-      <c r="BP24" s="78"/>
-      <c r="BQ24" s="79"/>
-      <c r="BR24" s="77"/>
-      <c r="BS24" s="78"/>
-      <c r="BT24" s="79"/>
-      <c r="BU24" s="77"/>
-      <c r="BV24" s="78"/>
-      <c r="BW24" s="79"/>
-      <c r="BX24" s="77"/>
-      <c r="BY24" s="78"/>
-      <c r="BZ24" s="79"/>
-      <c r="CA24" s="77"/>
-      <c r="CB24" s="78"/>
-      <c r="CC24" s="79"/>
-      <c r="CD24" s="77"/>
-      <c r="CE24" s="78"/>
-      <c r="CF24" s="79"/>
-      <c r="CG24" s="77"/>
-      <c r="CH24" s="78"/>
-      <c r="CI24" s="79"/>
-      <c r="CJ24" s="77"/>
-      <c r="CK24" s="78"/>
-      <c r="CL24" s="79"/>
-      <c r="CM24" s="77"/>
-      <c r="CN24" s="78"/>
-      <c r="CO24" s="79"/>
-      <c r="CP24" s="77"/>
-      <c r="CQ24" s="78"/>
-      <c r="CR24" s="79"/>
-      <c r="CS24" s="77"/>
-      <c r="CT24" s="78"/>
-      <c r="CU24" s="79"/>
-      <c r="CV24" s="77"/>
-      <c r="CW24" s="78"/>
-      <c r="CX24" s="79"/>
-      <c r="CY24" s="77"/>
-      <c r="CZ24" s="78"/>
-      <c r="DA24" s="79"/>
-      <c r="DB24" s="77"/>
-      <c r="DC24" s="78"/>
-      <c r="DD24" s="79"/>
-      <c r="DE24" s="77"/>
-      <c r="DF24" s="78"/>
-      <c r="DG24" s="79"/>
-      <c r="DH24" s="77"/>
-      <c r="DI24" s="78"/>
-      <c r="DJ24" s="79"/>
-      <c r="DK24" s="77"/>
-      <c r="DL24" s="78"/>
-      <c r="DM24" s="79"/>
-      <c r="DN24" s="77"/>
-      <c r="DO24" s="78"/>
-      <c r="DP24" s="79"/>
-      <c r="DQ24" s="77"/>
-      <c r="DR24" s="78"/>
-      <c r="DS24" s="79"/>
-      <c r="DT24" s="77"/>
-      <c r="DU24" s="78"/>
-      <c r="DV24" s="79"/>
-      <c r="DW24" s="77"/>
-      <c r="DX24" s="78"/>
-      <c r="DY24" s="79"/>
-      <c r="DZ24" s="77"/>
-      <c r="EA24" s="78"/>
-      <c r="EB24" s="79"/>
-      <c r="EC24" s="77"/>
-      <c r="ED24" s="78"/>
-      <c r="EE24" s="79"/>
-      <c r="EF24" s="77"/>
-      <c r="EG24" s="78"/>
-      <c r="EH24" s="79"/>
-      <c r="EI24" s="77"/>
-      <c r="EJ24" s="78"/>
-      <c r="EK24" s="79"/>
-      <c r="EL24" s="77"/>
-      <c r="EM24" s="78"/>
-      <c r="EN24" s="79"/>
-      <c r="EO24" s="77"/>
-      <c r="EP24" s="78"/>
-      <c r="EQ24" s="79"/>
-      <c r="ER24" s="77"/>
-      <c r="ES24" s="78"/>
-      <c r="ET24" s="79"/>
-      <c r="EU24" s="77"/>
-      <c r="EV24" s="78"/>
-      <c r="EW24" s="79"/>
-      <c r="EX24" s="77"/>
-      <c r="EY24" s="78"/>
-      <c r="EZ24" s="79"/>
-      <c r="FA24" s="77"/>
-      <c r="FB24" s="78"/>
-      <c r="FC24" s="79"/>
-      <c r="FD24" s="77"/>
-      <c r="FE24" s="78"/>
-      <c r="FF24" s="79"/>
-      <c r="FG24" s="77"/>
-      <c r="FH24" s="78"/>
-      <c r="FI24" s="79"/>
-      <c r="FJ24" s="77"/>
-      <c r="FK24" s="78"/>
-      <c r="FL24" s="79"/>
-      <c r="FM24" s="77"/>
-      <c r="FN24" s="78"/>
-      <c r="FO24" s="79"/>
-      <c r="FP24" s="77"/>
-      <c r="FQ24" s="78"/>
-      <c r="FR24" s="79"/>
-      <c r="FS24" s="77"/>
-      <c r="FT24" s="78"/>
-      <c r="FU24" s="79"/>
-      <c r="FV24" s="77"/>
-      <c r="FW24" s="78"/>
-      <c r="FX24" s="79"/>
-      <c r="FY24" s="77"/>
-      <c r="FZ24" s="78"/>
-      <c r="GA24" s="79"/>
-      <c r="GB24" s="77"/>
-      <c r="GC24" s="78"/>
-      <c r="GD24" s="79"/>
-      <c r="GE24" s="77"/>
-      <c r="GF24" s="78"/>
-      <c r="GG24" s="79"/>
+      <c r="D24" s="90"/>
+      <c r="E24" s="91"/>
+      <c r="F24" s="92"/>
+      <c r="G24" s="90"/>
+      <c r="H24" s="91"/>
+      <c r="I24" s="92"/>
+      <c r="J24" s="90"/>
+      <c r="K24" s="91"/>
+      <c r="L24" s="92"/>
+      <c r="M24" s="90"/>
+      <c r="N24" s="91"/>
+      <c r="O24" s="92"/>
+      <c r="P24" s="90"/>
+      <c r="Q24" s="91"/>
+      <c r="R24" s="92"/>
+      <c r="S24" s="90"/>
+      <c r="T24" s="91"/>
+      <c r="U24" s="92"/>
+      <c r="V24" s="90"/>
+      <c r="W24" s="91"/>
+      <c r="X24" s="92"/>
+      <c r="Y24" s="90"/>
+      <c r="Z24" s="91"/>
+      <c r="AA24" s="92"/>
+      <c r="AB24" s="90"/>
+      <c r="AC24" s="91"/>
+      <c r="AD24" s="92"/>
+      <c r="AE24" s="90"/>
+      <c r="AF24" s="91"/>
+      <c r="AG24" s="92"/>
+      <c r="AH24" s="90"/>
+      <c r="AI24" s="91"/>
+      <c r="AJ24" s="92"/>
+      <c r="AK24" s="90"/>
+      <c r="AL24" s="91"/>
+      <c r="AM24" s="92"/>
+      <c r="AN24" s="90"/>
+      <c r="AO24" s="91"/>
+      <c r="AP24" s="92"/>
+      <c r="AQ24" s="90"/>
+      <c r="AR24" s="91"/>
+      <c r="AS24" s="92"/>
+      <c r="AT24" s="90"/>
+      <c r="AU24" s="91"/>
+      <c r="AV24" s="92"/>
+      <c r="AW24" s="90"/>
+      <c r="AX24" s="91"/>
+      <c r="AY24" s="92"/>
+      <c r="AZ24" s="90"/>
+      <c r="BA24" s="91"/>
+      <c r="BB24" s="92"/>
+      <c r="BC24" s="90"/>
+      <c r="BD24" s="91"/>
+      <c r="BE24" s="92"/>
+      <c r="BF24" s="90"/>
+      <c r="BG24" s="91"/>
+      <c r="BH24" s="92"/>
+      <c r="BI24" s="90"/>
+      <c r="BJ24" s="91"/>
+      <c r="BK24" s="92"/>
+      <c r="BL24" s="90"/>
+      <c r="BM24" s="91"/>
+      <c r="BN24" s="92"/>
+      <c r="BO24" s="90"/>
+      <c r="BP24" s="91"/>
+      <c r="BQ24" s="92"/>
+      <c r="BR24" s="90"/>
+      <c r="BS24" s="91"/>
+      <c r="BT24" s="92"/>
+      <c r="BU24" s="90"/>
+      <c r="BV24" s="91"/>
+      <c r="BW24" s="92"/>
+      <c r="BX24" s="90"/>
+      <c r="BY24" s="91"/>
+      <c r="BZ24" s="92"/>
+      <c r="CA24" s="90"/>
+      <c r="CB24" s="91"/>
+      <c r="CC24" s="92"/>
+      <c r="CD24" s="90"/>
+      <c r="CE24" s="91"/>
+      <c r="CF24" s="92"/>
+      <c r="CG24" s="90"/>
+      <c r="CH24" s="91"/>
+      <c r="CI24" s="92"/>
+      <c r="CJ24" s="90"/>
+      <c r="CK24" s="91"/>
+      <c r="CL24" s="92"/>
+      <c r="CM24" s="90"/>
+      <c r="CN24" s="91"/>
+      <c r="CO24" s="92"/>
+      <c r="CP24" s="90"/>
+      <c r="CQ24" s="91"/>
+      <c r="CR24" s="92"/>
+      <c r="CS24" s="90"/>
+      <c r="CT24" s="91"/>
+      <c r="CU24" s="92"/>
+      <c r="CV24" s="90"/>
+      <c r="CW24" s="91"/>
+      <c r="CX24" s="92"/>
+      <c r="CY24" s="90"/>
+      <c r="CZ24" s="91"/>
+      <c r="DA24" s="92"/>
+      <c r="DB24" s="90"/>
+      <c r="DC24" s="91"/>
+      <c r="DD24" s="92"/>
+      <c r="DE24" s="90"/>
+      <c r="DF24" s="91"/>
+      <c r="DG24" s="92"/>
+      <c r="DH24" s="90"/>
+      <c r="DI24" s="91"/>
+      <c r="DJ24" s="92"/>
+      <c r="DK24" s="90"/>
+      <c r="DL24" s="91"/>
+      <c r="DM24" s="92"/>
+      <c r="DN24" s="90"/>
+      <c r="DO24" s="91"/>
+      <c r="DP24" s="92"/>
+      <c r="DQ24" s="90"/>
+      <c r="DR24" s="91"/>
+      <c r="DS24" s="92"/>
+      <c r="DT24" s="90"/>
+      <c r="DU24" s="91"/>
+      <c r="DV24" s="92"/>
+      <c r="DW24" s="90"/>
+      <c r="DX24" s="91"/>
+      <c r="DY24" s="92"/>
+      <c r="DZ24" s="90"/>
+      <c r="EA24" s="91"/>
+      <c r="EB24" s="92"/>
+      <c r="EC24" s="90"/>
+      <c r="ED24" s="91"/>
+      <c r="EE24" s="92"/>
+      <c r="EF24" s="90"/>
+      <c r="EG24" s="91"/>
+      <c r="EH24" s="92"/>
+      <c r="EI24" s="90"/>
+      <c r="EJ24" s="91"/>
+      <c r="EK24" s="92"/>
+      <c r="EL24" s="90"/>
+      <c r="EM24" s="91"/>
+      <c r="EN24" s="92"/>
+      <c r="EO24" s="90"/>
+      <c r="EP24" s="91"/>
+      <c r="EQ24" s="92"/>
+      <c r="ER24" s="90"/>
+      <c r="ES24" s="91"/>
+      <c r="ET24" s="92"/>
+      <c r="EU24" s="90"/>
+      <c r="EV24" s="91"/>
+      <c r="EW24" s="92"/>
+      <c r="EX24" s="90"/>
+      <c r="EY24" s="91"/>
+      <c r="EZ24" s="92"/>
+      <c r="FA24" s="90"/>
+      <c r="FB24" s="91"/>
+      <c r="FC24" s="92"/>
+      <c r="FD24" s="90"/>
+      <c r="FE24" s="91"/>
+      <c r="FF24" s="92"/>
+      <c r="FG24" s="90"/>
+      <c r="FH24" s="91"/>
+      <c r="FI24" s="92"/>
+      <c r="FJ24" s="90"/>
+      <c r="FK24" s="91"/>
+      <c r="FL24" s="92"/>
+      <c r="FM24" s="90"/>
+      <c r="FN24" s="91"/>
+      <c r="FO24" s="92"/>
+      <c r="FP24" s="90"/>
+      <c r="FQ24" s="91"/>
+      <c r="FR24" s="92"/>
+      <c r="FS24" s="90"/>
+      <c r="FT24" s="91"/>
+      <c r="FU24" s="92"/>
+      <c r="FV24" s="90"/>
+      <c r="FW24" s="91"/>
+      <c r="FX24" s="92"/>
+      <c r="FY24" s="90"/>
+      <c r="FZ24" s="91"/>
+      <c r="GA24" s="92"/>
+      <c r="GB24" s="90"/>
+      <c r="GC24" s="91"/>
+      <c r="GD24" s="92"/>
+      <c r="GE24" s="90"/>
+      <c r="GF24" s="91"/>
+      <c r="GG24" s="92"/>
     </row>
     <row r="25" spans="1:291" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
@@ -13857,8 +13834,8 @@
       </c>
     </row>
     <row r="26" spans="1:291" x14ac:dyDescent="0.25">
-      <c r="A26" s="76"/>
-      <c r="B26" s="76"/>
+      <c r="A26" s="74"/>
+      <c r="B26" s="74"/>
       <c r="C26" s="8" t="s">
         <v>23</v>
       </c>
@@ -14050,8 +14027,8 @@
       <c r="GG26" s="56"/>
     </row>
     <row r="27" spans="1:291" x14ac:dyDescent="0.25">
-      <c r="A27" s="75"/>
-      <c r="B27" s="75"/>
+      <c r="A27" s="73"/>
+      <c r="B27" s="73"/>
       <c r="C27" s="39" t="s">
         <v>24</v>
       </c>
@@ -14243,8 +14220,8 @@
       <c r="GG27" s="56"/>
     </row>
     <row r="28" spans="1:291" x14ac:dyDescent="0.25">
-      <c r="A28" s="76"/>
-      <c r="B28" s="76"/>
+      <c r="A28" s="74"/>
+      <c r="B28" s="74"/>
       <c r="C28" s="8" t="s">
         <v>23</v>
       </c>
@@ -14436,8 +14413,8 @@
       <c r="GG28" s="56"/>
     </row>
     <row r="29" spans="1:291" x14ac:dyDescent="0.25">
-      <c r="A29" s="75"/>
-      <c r="B29" s="75"/>
+      <c r="A29" s="73"/>
+      <c r="B29" s="73"/>
       <c r="C29" s="39" t="s">
         <v>24</v>
       </c>
@@ -14629,8 +14606,8 @@
       <c r="GG29" s="56"/>
     </row>
     <row r="30" spans="1:291" x14ac:dyDescent="0.25">
-      <c r="A30" s="76"/>
-      <c r="B30" s="76"/>
+      <c r="A30" s="74"/>
+      <c r="B30" s="74"/>
       <c r="C30" s="8" t="s">
         <v>23</v>
       </c>
@@ -14822,8 +14799,8 @@
       <c r="GG30" s="56"/>
     </row>
     <row r="31" spans="1:291" x14ac:dyDescent="0.25">
-      <c r="A31" s="75"/>
-      <c r="B31" s="75"/>
+      <c r="A31" s="73"/>
+      <c r="B31" s="73"/>
       <c r="C31" s="39" t="s">
         <v>24</v>
       </c>
@@ -15015,8 +14992,8 @@
       <c r="GG31" s="56"/>
     </row>
     <row r="32" spans="1:291" x14ac:dyDescent="0.25">
-      <c r="A32" s="76"/>
-      <c r="B32" s="76"/>
+      <c r="A32" s="74"/>
+      <c r="B32" s="74"/>
       <c r="C32" s="8" t="s">
         <v>23</v>
       </c>
@@ -15208,8 +15185,8 @@
       <c r="GG32" s="56"/>
     </row>
     <row r="33" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A33" s="75"/>
-      <c r="B33" s="75"/>
+      <c r="A33" s="73"/>
+      <c r="B33" s="73"/>
       <c r="C33" s="39" t="s">
         <v>24</v>
       </c>
@@ -15401,8 +15378,8 @@
       <c r="GG33" s="56"/>
     </row>
     <row r="34" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A34" s="76"/>
-      <c r="B34" s="76"/>
+      <c r="A34" s="74"/>
+      <c r="B34" s="74"/>
       <c r="C34" s="8" t="s">
         <v>23</v>
       </c>
@@ -15594,8 +15571,8 @@
       <c r="GG34" s="58"/>
     </row>
     <row r="35" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A35" s="75"/>
-      <c r="B35" s="75"/>
+      <c r="A35" s="73"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="39" t="s">
         <v>24</v>
       </c>
@@ -15787,8 +15764,8 @@
       <c r="GG35" s="56"/>
     </row>
     <row r="36" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A36" s="76"/>
-      <c r="B36" s="76"/>
+      <c r="A36" s="74"/>
+      <c r="B36" s="74"/>
       <c r="C36" s="8" t="s">
         <v>23</v>
       </c>
@@ -15980,8 +15957,8 @@
       <c r="GG36" s="56"/>
     </row>
     <row r="37" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A37" s="75"/>
-      <c r="B37" s="75"/>
+      <c r="A37" s="73"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="39" t="s">
         <v>24</v>
       </c>
@@ -16173,8 +16150,8 @@
       <c r="GG37" s="58"/>
     </row>
     <row r="38" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A38" s="76"/>
-      <c r="B38" s="76"/>
+      <c r="A38" s="74"/>
+      <c r="B38" s="74"/>
       <c r="C38" s="8" t="s">
         <v>23</v>
       </c>
@@ -16366,8 +16343,8 @@
       <c r="GG38" s="58"/>
     </row>
     <row r="39" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A39" s="75"/>
-      <c r="B39" s="75"/>
+      <c r="A39" s="73"/>
+      <c r="B39" s="73"/>
       <c r="C39" s="39" t="s">
         <v>24</v>
       </c>
@@ -16559,8 +16536,8 @@
       <c r="GG39" s="56"/>
     </row>
     <row r="40" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A40" s="76"/>
-      <c r="B40" s="76"/>
+      <c r="A40" s="74"/>
+      <c r="B40" s="74"/>
       <c r="C40" s="8" t="s">
         <v>23</v>
       </c>
@@ -16752,8 +16729,8 @@
       <c r="GG40" s="58"/>
     </row>
     <row r="41" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A41" s="75"/>
-      <c r="B41" s="75"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="73"/>
       <c r="C41" s="39" t="s">
         <v>24</v>
       </c>
@@ -16945,8 +16922,8 @@
       <c r="GG41" s="56"/>
     </row>
     <row r="42" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A42" s="76"/>
-      <c r="B42" s="76"/>
+      <c r="A42" s="74"/>
+      <c r="B42" s="74"/>
       <c r="C42" s="8" t="s">
         <v>23</v>
       </c>
@@ -17138,8 +17115,8 @@
       <c r="GG42" s="58"/>
     </row>
     <row r="43" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A43" s="75"/>
-      <c r="B43" s="75"/>
+      <c r="A43" s="73"/>
+      <c r="B43" s="73"/>
       <c r="C43" s="39" t="s">
         <v>24</v>
       </c>
@@ -17331,8 +17308,8 @@
       <c r="GG43" s="56"/>
     </row>
     <row r="44" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A44" s="76"/>
-      <c r="B44" s="76"/>
+      <c r="A44" s="74"/>
+      <c r="B44" s="74"/>
       <c r="C44" s="8" t="s">
         <v>23</v>
       </c>
@@ -17524,8 +17501,8 @@
       <c r="GG44" s="58"/>
     </row>
     <row r="45" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A45" s="75"/>
-      <c r="B45" s="75"/>
+      <c r="A45" s="73"/>
+      <c r="B45" s="73"/>
       <c r="C45" s="39" t="s">
         <v>24</v>
       </c>
@@ -17717,8 +17694,8 @@
       <c r="GG45" s="56"/>
     </row>
     <row r="46" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A46" s="76"/>
-      <c r="B46" s="76"/>
+      <c r="A46" s="74"/>
+      <c r="B46" s="74"/>
       <c r="C46" s="8" t="s">
         <v>23</v>
       </c>
@@ -17910,8 +17887,8 @@
       <c r="GG46" s="58"/>
     </row>
     <row r="47" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A47" s="75"/>
-      <c r="B47" s="75"/>
+      <c r="A47" s="73"/>
+      <c r="B47" s="73"/>
       <c r="C47" s="39" t="s">
         <v>24</v>
       </c>
@@ -18103,8 +18080,8 @@
       <c r="GG47" s="56"/>
     </row>
     <row r="48" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A48" s="76"/>
-      <c r="B48" s="76"/>
+      <c r="A48" s="74"/>
+      <c r="B48" s="74"/>
       <c r="C48" s="8" t="s">
         <v>23</v>
       </c>
@@ -18296,8 +18273,8 @@
       <c r="GG48" s="58"/>
     </row>
     <row r="49" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A49" s="75"/>
-      <c r="B49" s="75"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="73"/>
       <c r="C49" s="39" t="s">
         <v>24</v>
       </c>
@@ -18489,8 +18466,8 @@
       <c r="GG49" s="56"/>
     </row>
     <row r="50" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A50" s="74"/>
-      <c r="B50" s="76"/>
+      <c r="A50" s="72"/>
+      <c r="B50" s="74"/>
       <c r="C50" s="8" t="s">
         <v>23</v>
       </c>
@@ -18682,8 +18659,8 @@
       <c r="GG50" s="58"/>
     </row>
     <row r="51" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A51" s="75"/>
-      <c r="B51" s="75"/>
+      <c r="A51" s="73"/>
+      <c r="B51" s="73"/>
       <c r="C51" s="39" t="s">
         <v>24</v>
       </c>
@@ -18875,8 +18852,8 @@
       <c r="GG51" s="58"/>
     </row>
     <row r="52" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A52" s="74"/>
-      <c r="B52" s="76"/>
+      <c r="A52" s="72"/>
+      <c r="B52" s="74"/>
       <c r="C52" s="8" t="s">
         <v>23</v>
       </c>
@@ -19068,8 +19045,8 @@
       <c r="GG52" s="58"/>
     </row>
     <row r="53" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A53" s="75"/>
-      <c r="B53" s="75"/>
+      <c r="A53" s="73"/>
+      <c r="B53" s="73"/>
       <c r="C53" s="39" t="s">
         <v>24</v>
       </c>
@@ -19261,8 +19238,8 @@
       <c r="GG53" s="58"/>
     </row>
     <row r="54" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A54" s="74"/>
-      <c r="B54" s="76"/>
+      <c r="A54" s="72"/>
+      <c r="B54" s="74"/>
       <c r="C54" s="8" t="s">
         <v>23</v>
       </c>
@@ -19454,8 +19431,8 @@
       <c r="GG54" s="58"/>
     </row>
     <row r="55" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A55" s="75"/>
-      <c r="B55" s="75"/>
+      <c r="A55" s="73"/>
+      <c r="B55" s="73"/>
       <c r="C55" s="39" t="s">
         <v>24</v>
       </c>
@@ -19647,8 +19624,8 @@
       <c r="GG55" s="58"/>
     </row>
     <row r="56" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A56" s="74"/>
-      <c r="B56" s="76"/>
+      <c r="A56" s="72"/>
+      <c r="B56" s="74"/>
       <c r="C56" s="8" t="s">
         <v>23</v>
       </c>
@@ -19840,8 +19817,8 @@
       <c r="GG56" s="58"/>
     </row>
     <row r="57" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A57" s="75"/>
-      <c r="B57" s="75"/>
+      <c r="A57" s="73"/>
+      <c r="B57" s="73"/>
       <c r="C57" s="39" t="s">
         <v>24</v>
       </c>
@@ -20033,8 +20010,8 @@
       <c r="GG57" s="58"/>
     </row>
     <row r="58" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A58" s="74"/>
-      <c r="B58" s="76"/>
+      <c r="A58" s="72"/>
+      <c r="B58" s="74"/>
       <c r="C58" s="8" t="s">
         <v>23</v>
       </c>
@@ -20226,8 +20203,8 @@
       <c r="GG58" s="58"/>
     </row>
     <row r="59" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A59" s="75"/>
-      <c r="B59" s="75"/>
+      <c r="A59" s="73"/>
+      <c r="B59" s="73"/>
       <c r="C59" s="39" t="s">
         <v>24</v>
       </c>
@@ -20419,8 +20396,8 @@
       <c r="GG59" s="58"/>
     </row>
     <row r="60" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A60" s="74"/>
-      <c r="B60" s="76"/>
+      <c r="A60" s="72"/>
+      <c r="B60" s="74"/>
       <c r="C60" s="8" t="s">
         <v>23</v>
       </c>
@@ -20612,8 +20589,8 @@
       <c r="GG60" s="58"/>
     </row>
     <row r="61" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A61" s="75"/>
-      <c r="B61" s="75"/>
+      <c r="A61" s="73"/>
+      <c r="B61" s="73"/>
       <c r="C61" s="39" t="s">
         <v>24</v>
       </c>
@@ -20805,8 +20782,8 @@
       <c r="GG61" s="58"/>
     </row>
     <row r="62" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A62" s="74"/>
-      <c r="B62" s="76"/>
+      <c r="A62" s="72"/>
+      <c r="B62" s="74"/>
       <c r="C62" s="8" t="s">
         <v>23</v>
       </c>
@@ -20998,8 +20975,8 @@
       <c r="GG62" s="58"/>
     </row>
     <row r="63" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A63" s="75"/>
-      <c r="B63" s="75"/>
+      <c r="A63" s="73"/>
+      <c r="B63" s="73"/>
       <c r="C63" s="39" t="s">
         <v>24</v>
       </c>
@@ -21191,8 +21168,8 @@
       <c r="GG63" s="58"/>
     </row>
     <row r="64" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A64" s="74"/>
-      <c r="B64" s="76"/>
+      <c r="A64" s="72"/>
+      <c r="B64" s="74"/>
       <c r="C64" s="8" t="s">
         <v>23</v>
       </c>
@@ -21384,8 +21361,8 @@
       <c r="GG64" s="58"/>
     </row>
     <row r="65" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A65" s="75"/>
-      <c r="B65" s="75"/>
+      <c r="A65" s="73"/>
+      <c r="B65" s="73"/>
       <c r="C65" s="39" t="s">
         <v>24</v>
       </c>
@@ -21577,8 +21554,8 @@
       <c r="GG65" s="58"/>
     </row>
     <row r="66" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A66" s="74"/>
-      <c r="B66" s="76"/>
+      <c r="A66" s="72"/>
+      <c r="B66" s="74"/>
       <c r="C66" s="8" t="s">
         <v>23</v>
       </c>
@@ -21770,8 +21747,8 @@
       <c r="GG66" s="58"/>
     </row>
     <row r="67" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A67" s="75"/>
-      <c r="B67" s="75"/>
+      <c r="A67" s="73"/>
+      <c r="B67" s="73"/>
       <c r="C67" s="39" t="s">
         <v>24</v>
       </c>
@@ -21963,8 +21940,8 @@
       <c r="GG67" s="58"/>
     </row>
     <row r="68" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A68" s="74"/>
-      <c r="B68" s="76"/>
+      <c r="A68" s="72"/>
+      <c r="B68" s="74"/>
       <c r="C68" s="8" t="s">
         <v>23</v>
       </c>
@@ -22156,8 +22133,8 @@
       <c r="GG68" s="58"/>
     </row>
     <row r="69" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A69" s="75"/>
-      <c r="B69" s="75"/>
+      <c r="A69" s="73"/>
+      <c r="B69" s="73"/>
       <c r="C69" s="39" t="s">
         <v>24</v>
       </c>
@@ -22349,8 +22326,8 @@
       <c r="GG69" s="58"/>
     </row>
     <row r="70" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A70" s="74"/>
-      <c r="B70" s="76"/>
+      <c r="A70" s="72"/>
+      <c r="B70" s="74"/>
       <c r="C70" s="8" t="s">
         <v>23</v>
       </c>
@@ -22542,8 +22519,8 @@
       <c r="GG70" s="58"/>
     </row>
     <row r="71" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A71" s="75"/>
-      <c r="B71" s="75"/>
+      <c r="A71" s="73"/>
+      <c r="B71" s="73"/>
       <c r="C71" s="39" t="s">
         <v>24</v>
       </c>
@@ -22735,8 +22712,8 @@
       <c r="GG71" s="58"/>
     </row>
     <row r="72" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A72" s="74"/>
-      <c r="B72" s="76"/>
+      <c r="A72" s="72"/>
+      <c r="B72" s="74"/>
       <c r="C72" s="8" t="s">
         <v>23</v>
       </c>
@@ -22928,8 +22905,8 @@
       <c r="GG72" s="58"/>
     </row>
     <row r="73" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A73" s="75"/>
-      <c r="B73" s="75"/>
+      <c r="A73" s="73"/>
+      <c r="B73" s="73"/>
       <c r="C73" s="39" t="s">
         <v>24</v>
       </c>
@@ -23121,8 +23098,8 @@
       <c r="GG73" s="58"/>
     </row>
     <row r="74" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A74" s="74"/>
-      <c r="B74" s="76"/>
+      <c r="A74" s="72"/>
+      <c r="B74" s="74"/>
       <c r="C74" s="8" t="s">
         <v>23</v>
       </c>
@@ -23314,8 +23291,8 @@
       <c r="GG74" s="58"/>
     </row>
     <row r="75" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A75" s="75"/>
-      <c r="B75" s="75"/>
+      <c r="A75" s="73"/>
+      <c r="B75" s="73"/>
       <c r="C75" s="39" t="s">
         <v>24</v>
       </c>
@@ -23507,8 +23484,8 @@
       <c r="GG75" s="58"/>
     </row>
     <row r="76" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A76" s="74"/>
-      <c r="B76" s="76"/>
+      <c r="A76" s="72"/>
+      <c r="B76" s="74"/>
       <c r="C76" s="8" t="s">
         <v>23</v>
       </c>
@@ -23700,8 +23677,8 @@
       <c r="GG76" s="58"/>
     </row>
     <row r="77" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A77" s="75"/>
-      <c r="B77" s="75"/>
+      <c r="A77" s="73"/>
+      <c r="B77" s="73"/>
       <c r="C77" s="39" t="s">
         <v>24</v>
       </c>
@@ -23893,8 +23870,8 @@
       <c r="GG77" s="58"/>
     </row>
     <row r="78" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A78" s="74"/>
-      <c r="B78" s="76"/>
+      <c r="A78" s="72"/>
+      <c r="B78" s="74"/>
       <c r="C78" s="8" t="s">
         <v>23</v>
       </c>
@@ -24086,8 +24063,8 @@
       <c r="GG78" s="58"/>
     </row>
     <row r="79" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A79" s="75"/>
-      <c r="B79" s="75"/>
+      <c r="A79" s="73"/>
+      <c r="B79" s="73"/>
       <c r="C79" s="39" t="s">
         <v>24</v>
       </c>
@@ -24279,8 +24256,8 @@
       <c r="GG79" s="58"/>
     </row>
     <row r="80" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A80" s="74"/>
-      <c r="B80" s="76"/>
+      <c r="A80" s="72"/>
+      <c r="B80" s="74"/>
       <c r="C80" s="8" t="s">
         <v>23</v>
       </c>
@@ -24472,8 +24449,8 @@
       <c r="GG80" s="58"/>
     </row>
     <row r="81" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A81" s="75"/>
-      <c r="B81" s="75"/>
+      <c r="A81" s="73"/>
+      <c r="B81" s="73"/>
       <c r="C81" s="39" t="s">
         <v>24</v>
       </c>
@@ -24665,8 +24642,8 @@
       <c r="GG81" s="58"/>
     </row>
     <row r="82" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A82" s="74"/>
-      <c r="B82" s="76"/>
+      <c r="A82" s="72"/>
+      <c r="B82" s="74"/>
       <c r="C82" s="8" t="s">
         <v>23</v>
       </c>
@@ -24858,8 +24835,8 @@
       <c r="GG82" s="58"/>
     </row>
     <row r="83" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A83" s="75"/>
-      <c r="B83" s="75"/>
+      <c r="A83" s="73"/>
+      <c r="B83" s="73"/>
       <c r="C83" s="39" t="s">
         <v>24</v>
       </c>
@@ -25051,8 +25028,8 @@
       <c r="GG83" s="58"/>
     </row>
     <row r="84" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A84" s="74"/>
-      <c r="B84" s="76"/>
+      <c r="A84" s="72"/>
+      <c r="B84" s="74"/>
       <c r="C84" s="8" t="s">
         <v>23</v>
       </c>
@@ -25244,8 +25221,8 @@
       <c r="GG84" s="58"/>
     </row>
     <row r="85" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A85" s="75"/>
-      <c r="B85" s="75"/>
+      <c r="A85" s="73"/>
+      <c r="B85" s="73"/>
       <c r="C85" s="39" t="s">
         <v>24</v>
       </c>
@@ -25437,8 +25414,8 @@
       <c r="GG85" s="58"/>
     </row>
     <row r="86" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A86" s="74"/>
-      <c r="B86" s="76"/>
+      <c r="A86" s="72"/>
+      <c r="B86" s="74"/>
       <c r="C86" s="8" t="s">
         <v>23</v>
       </c>
@@ -25630,8 +25607,8 @@
       <c r="GG86" s="58"/>
     </row>
     <row r="87" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A87" s="75"/>
-      <c r="B87" s="75"/>
+      <c r="A87" s="73"/>
+      <c r="B87" s="73"/>
       <c r="C87" s="39" t="s">
         <v>24</v>
       </c>
@@ -25823,8 +25800,8 @@
       <c r="GG87" s="58"/>
     </row>
     <row r="88" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A88" s="74"/>
-      <c r="B88" s="76"/>
+      <c r="A88" s="72"/>
+      <c r="B88" s="74"/>
       <c r="C88" s="8" t="s">
         <v>23</v>
       </c>
@@ -26016,8 +25993,8 @@
       <c r="GG88" s="58"/>
     </row>
     <row r="89" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A89" s="75"/>
-      <c r="B89" s="75"/>
+      <c r="A89" s="73"/>
+      <c r="B89" s="73"/>
       <c r="C89" s="39" t="s">
         <v>24</v>
       </c>
@@ -26209,8 +26186,8 @@
       <c r="GG89" s="58"/>
     </row>
     <row r="90" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A90" s="74"/>
-      <c r="B90" s="76"/>
+      <c r="A90" s="72"/>
+      <c r="B90" s="74"/>
       <c r="C90" s="8" t="s">
         <v>23</v>
       </c>
@@ -26402,8 +26379,8 @@
       <c r="GG90" s="58"/>
     </row>
     <row r="91" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A91" s="75"/>
-      <c r="B91" s="75"/>
+      <c r="A91" s="73"/>
+      <c r="B91" s="73"/>
       <c r="C91" s="39" t="s">
         <v>24</v>
       </c>
@@ -26595,8 +26572,8 @@
       <c r="GG91" s="58"/>
     </row>
     <row r="92" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A92" s="74"/>
-      <c r="B92" s="76"/>
+      <c r="A92" s="72"/>
+      <c r="B92" s="74"/>
       <c r="C92" s="8" t="s">
         <v>23</v>
       </c>
@@ -26788,8 +26765,8 @@
       <c r="GG92" s="58"/>
     </row>
     <row r="93" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A93" s="75"/>
-      <c r="B93" s="75"/>
+      <c r="A93" s="73"/>
+      <c r="B93" s="73"/>
       <c r="C93" s="39" t="s">
         <v>24</v>
       </c>
@@ -26981,8 +26958,8 @@
       <c r="GG93" s="58"/>
     </row>
     <row r="94" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A94" s="74"/>
-      <c r="B94" s="76"/>
+      <c r="A94" s="72"/>
+      <c r="B94" s="74"/>
       <c r="C94" s="8" t="s">
         <v>23</v>
       </c>
@@ -27174,8 +27151,8 @@
       <c r="GG94" s="58"/>
     </row>
     <row r="95" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A95" s="75"/>
-      <c r="B95" s="75"/>
+      <c r="A95" s="73"/>
+      <c r="B95" s="73"/>
       <c r="C95" s="39" t="s">
         <v>24</v>
       </c>
@@ -27367,8 +27344,8 @@
       <c r="GG95" s="58"/>
     </row>
     <row r="96" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A96" s="74"/>
-      <c r="B96" s="76"/>
+      <c r="A96" s="72"/>
+      <c r="B96" s="74"/>
       <c r="C96" s="8" t="s">
         <v>23</v>
       </c>
@@ -27560,8 +27537,8 @@
       <c r="GG96" s="58"/>
     </row>
     <row r="97" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A97" s="75"/>
-      <c r="B97" s="75"/>
+      <c r="A97" s="73"/>
+      <c r="B97" s="73"/>
       <c r="C97" s="39" t="s">
         <v>24</v>
       </c>
@@ -27753,8 +27730,8 @@
       <c r="GG97" s="58"/>
     </row>
     <row r="98" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A98" s="74"/>
-      <c r="B98" s="76"/>
+      <c r="A98" s="72"/>
+      <c r="B98" s="74"/>
       <c r="C98" s="8" t="s">
         <v>23</v>
       </c>
@@ -27946,8 +27923,8 @@
       <c r="GG98" s="58"/>
     </row>
     <row r="99" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A99" s="75"/>
-      <c r="B99" s="75"/>
+      <c r="A99" s="73"/>
+      <c r="B99" s="73"/>
       <c r="C99" s="39" t="s">
         <v>24</v>
       </c>
@@ -28139,8 +28116,8 @@
       <c r="GG99" s="58"/>
     </row>
     <row r="100" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A100" s="74"/>
-      <c r="B100" s="76"/>
+      <c r="A100" s="72"/>
+      <c r="B100" s="74"/>
       <c r="C100" s="8" t="s">
         <v>23</v>
       </c>
@@ -28332,8 +28309,8 @@
       <c r="GG100" s="58"/>
     </row>
     <row r="101" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A101" s="75"/>
-      <c r="B101" s="75"/>
+      <c r="A101" s="73"/>
+      <c r="B101" s="73"/>
       <c r="C101" s="39" t="s">
         <v>24</v>
       </c>
@@ -28525,8 +28502,8 @@
       <c r="GG101" s="58"/>
     </row>
     <row r="102" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A102" s="74"/>
-      <c r="B102" s="76"/>
+      <c r="A102" s="72"/>
+      <c r="B102" s="74"/>
       <c r="C102" s="8" t="s">
         <v>23</v>
       </c>
@@ -28718,8 +28695,8 @@
       <c r="GG102" s="58"/>
     </row>
     <row r="103" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A103" s="75"/>
-      <c r="B103" s="75"/>
+      <c r="A103" s="73"/>
+      <c r="B103" s="73"/>
       <c r="C103" s="39" t="s">
         <v>24</v>
       </c>
@@ -28911,8 +28888,8 @@
       <c r="GG103" s="58"/>
     </row>
     <row r="104" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A104" s="74"/>
-      <c r="B104" s="76"/>
+      <c r="A104" s="72"/>
+      <c r="B104" s="74"/>
       <c r="C104" s="8" t="s">
         <v>23</v>
       </c>
@@ -29104,8 +29081,8 @@
       <c r="GG104" s="58"/>
     </row>
     <row r="105" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A105" s="75"/>
-      <c r="B105" s="75"/>
+      <c r="A105" s="73"/>
+      <c r="B105" s="73"/>
       <c r="C105" s="39" t="s">
         <v>24</v>
       </c>
@@ -29297,8 +29274,8 @@
       <c r="GG105" s="58"/>
     </row>
     <row r="106" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A106" s="74"/>
-      <c r="B106" s="76"/>
+      <c r="A106" s="72"/>
+      <c r="B106" s="74"/>
       <c r="C106" s="8" t="s">
         <v>23</v>
       </c>
@@ -29490,8 +29467,8 @@
       <c r="GG106" s="58"/>
     </row>
     <row r="107" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A107" s="75"/>
-      <c r="B107" s="75"/>
+      <c r="A107" s="73"/>
+      <c r="B107" s="73"/>
       <c r="C107" s="39" t="s">
         <v>24</v>
       </c>
@@ -29683,8 +29660,8 @@
       <c r="GG107" s="58"/>
     </row>
     <row r="108" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A108" s="74"/>
-      <c r="B108" s="76"/>
+      <c r="A108" s="72"/>
+      <c r="B108" s="74"/>
       <c r="C108" s="8" t="s">
         <v>23</v>
       </c>
@@ -29876,8 +29853,8 @@
       <c r="GG108" s="58"/>
     </row>
     <row r="109" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A109" s="75"/>
-      <c r="B109" s="75"/>
+      <c r="A109" s="73"/>
+      <c r="B109" s="73"/>
       <c r="C109" s="39" t="s">
         <v>24</v>
       </c>
@@ -30069,8 +30046,8 @@
       <c r="GG109" s="58"/>
     </row>
     <row r="110" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A110" s="74"/>
-      <c r="B110" s="76"/>
+      <c r="A110" s="72"/>
+      <c r="B110" s="74"/>
       <c r="C110" s="8" t="s">
         <v>23</v>
       </c>
@@ -30262,8 +30239,8 @@
       <c r="GG110" s="58"/>
     </row>
     <row r="111" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A111" s="75"/>
-      <c r="B111" s="75"/>
+      <c r="A111" s="73"/>
+      <c r="B111" s="73"/>
       <c r="C111" s="39" t="s">
         <v>24</v>
       </c>
@@ -30455,8 +30432,8 @@
       <c r="GG111" s="58"/>
     </row>
     <row r="112" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A112" s="74"/>
-      <c r="B112" s="76"/>
+      <c r="A112" s="72"/>
+      <c r="B112" s="74"/>
       <c r="C112" s="8" t="s">
         <v>23</v>
       </c>
@@ -30648,8 +30625,8 @@
       <c r="GG112" s="58"/>
     </row>
     <row r="113" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A113" s="75"/>
-      <c r="B113" s="75"/>
+      <c r="A113" s="73"/>
+      <c r="B113" s="73"/>
       <c r="C113" s="39" t="s">
         <v>24</v>
       </c>
@@ -30841,8 +30818,8 @@
       <c r="GG113" s="58"/>
     </row>
     <row r="114" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A114" s="74"/>
-      <c r="B114" s="76"/>
+      <c r="A114" s="72"/>
+      <c r="B114" s="74"/>
       <c r="C114" s="8" t="s">
         <v>23</v>
       </c>
@@ -31034,8 +31011,8 @@
       <c r="GG114" s="58"/>
     </row>
     <row r="115" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A115" s="75"/>
-      <c r="B115" s="75"/>
+      <c r="A115" s="73"/>
+      <c r="B115" s="73"/>
       <c r="C115" s="39" t="s">
         <v>24</v>
       </c>
@@ -31227,8 +31204,8 @@
       <c r="GG115" s="58"/>
     </row>
     <row r="116" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A116" s="74"/>
-      <c r="B116" s="76"/>
+      <c r="A116" s="72"/>
+      <c r="B116" s="74"/>
       <c r="C116" s="8" t="s">
         <v>23</v>
       </c>
@@ -31420,8 +31397,8 @@
       <c r="GG116" s="58"/>
     </row>
     <row r="117" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A117" s="75"/>
-      <c r="B117" s="75"/>
+      <c r="A117" s="73"/>
+      <c r="B117" s="73"/>
       <c r="C117" s="39" t="s">
         <v>24</v>
       </c>
@@ -31613,8 +31590,8 @@
       <c r="GG117" s="58"/>
     </row>
     <row r="118" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A118" s="74"/>
-      <c r="B118" s="76"/>
+      <c r="A118" s="72"/>
+      <c r="B118" s="74"/>
       <c r="C118" s="8" t="s">
         <v>23</v>
       </c>
@@ -31806,8 +31783,8 @@
       <c r="GG118" s="58"/>
     </row>
     <row r="119" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A119" s="75"/>
-      <c r="B119" s="75"/>
+      <c r="A119" s="73"/>
+      <c r="B119" s="73"/>
       <c r="C119" s="39" t="s">
         <v>24</v>
       </c>
@@ -31999,8 +31976,8 @@
       <c r="GG119" s="58"/>
     </row>
     <row r="120" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A120" s="74"/>
-      <c r="B120" s="76"/>
+      <c r="A120" s="72"/>
+      <c r="B120" s="74"/>
       <c r="C120" s="8" t="s">
         <v>23</v>
       </c>
@@ -32192,8 +32169,8 @@
       <c r="GG120" s="58"/>
     </row>
     <row r="121" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A121" s="75"/>
-      <c r="B121" s="75"/>
+      <c r="A121" s="73"/>
+      <c r="B121" s="73"/>
       <c r="C121" s="39" t="s">
         <v>24</v>
       </c>
@@ -32385,8 +32362,8 @@
       <c r="GG121" s="58"/>
     </row>
     <row r="122" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A122" s="74"/>
-      <c r="B122" s="76"/>
+      <c r="A122" s="72"/>
+      <c r="B122" s="74"/>
       <c r="C122" s="8" t="s">
         <v>23</v>
       </c>
@@ -32578,8 +32555,8 @@
       <c r="GG122" s="58"/>
     </row>
     <row r="123" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A123" s="75"/>
-      <c r="B123" s="75"/>
+      <c r="A123" s="73"/>
+      <c r="B123" s="73"/>
       <c r="C123" s="39" t="s">
         <v>24</v>
       </c>
@@ -32771,8 +32748,8 @@
       <c r="GG123" s="58"/>
     </row>
     <row r="124" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A124" s="74"/>
-      <c r="B124" s="76"/>
+      <c r="A124" s="72"/>
+      <c r="B124" s="74"/>
       <c r="C124" s="8" t="s">
         <v>23</v>
       </c>
@@ -32964,8 +32941,8 @@
       <c r="GG124" s="58"/>
     </row>
     <row r="125" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A125" s="75"/>
-      <c r="B125" s="75"/>
+      <c r="A125" s="73"/>
+      <c r="B125" s="73"/>
       <c r="C125" s="39" t="s">
         <v>24</v>
       </c>
@@ -33157,8 +33134,8 @@
       <c r="GG125" s="58"/>
     </row>
     <row r="126" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A126" s="74"/>
-      <c r="B126" s="76"/>
+      <c r="A126" s="72"/>
+      <c r="B126" s="74"/>
       <c r="C126" s="8" t="s">
         <v>23</v>
       </c>
@@ -33350,8 +33327,8 @@
       <c r="GG126" s="58"/>
     </row>
     <row r="127" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A127" s="75"/>
-      <c r="B127" s="75"/>
+      <c r="A127" s="73"/>
+      <c r="B127" s="73"/>
       <c r="C127" s="39" t="s">
         <v>24</v>
       </c>
@@ -33543,8 +33520,8 @@
       <c r="GG127" s="58"/>
     </row>
     <row r="128" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A128" s="74"/>
-      <c r="B128" s="76"/>
+      <c r="A128" s="72"/>
+      <c r="B128" s="74"/>
       <c r="C128" s="8" t="s">
         <v>23</v>
       </c>
@@ -33736,8 +33713,8 @@
       <c r="GG128" s="58"/>
     </row>
     <row r="129" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A129" s="75"/>
-      <c r="B129" s="75"/>
+      <c r="A129" s="73"/>
+      <c r="B129" s="73"/>
       <c r="C129" s="39" t="s">
         <v>24</v>
       </c>
@@ -33929,8 +33906,8 @@
       <c r="GG129" s="58"/>
     </row>
     <row r="130" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A130" s="74"/>
-      <c r="B130" s="76"/>
+      <c r="A130" s="72"/>
+      <c r="B130" s="74"/>
       <c r="C130" s="8" t="s">
         <v>23</v>
       </c>
@@ -34122,8 +34099,8 @@
       <c r="GG130" s="58"/>
     </row>
     <row r="131" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A131" s="75"/>
-      <c r="B131" s="75"/>
+      <c r="A131" s="73"/>
+      <c r="B131" s="73"/>
       <c r="C131" s="39" t="s">
         <v>24</v>
       </c>
@@ -34315,8 +34292,8 @@
       <c r="GG131" s="58"/>
     </row>
     <row r="132" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A132" s="74"/>
-      <c r="B132" s="76"/>
+      <c r="A132" s="72"/>
+      <c r="B132" s="74"/>
       <c r="C132" s="8" t="s">
         <v>23</v>
       </c>
@@ -34508,8 +34485,8 @@
       <c r="GG132" s="58"/>
     </row>
     <row r="133" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A133" s="75"/>
-      <c r="B133" s="75"/>
+      <c r="A133" s="73"/>
+      <c r="B133" s="73"/>
       <c r="C133" s="39" t="s">
         <v>24</v>
       </c>
@@ -34701,8 +34678,8 @@
       <c r="GG133" s="58"/>
     </row>
     <row r="134" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A134" s="74"/>
-      <c r="B134" s="76"/>
+      <c r="A134" s="72"/>
+      <c r="B134" s="74"/>
       <c r="C134" s="8" t="s">
         <v>23</v>
       </c>
@@ -34894,8 +34871,8 @@
       <c r="GG134" s="58"/>
     </row>
     <row r="135" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A135" s="75"/>
-      <c r="B135" s="75"/>
+      <c r="A135" s="73"/>
+      <c r="B135" s="73"/>
       <c r="C135" s="39" t="s">
         <v>24</v>
       </c>
@@ -35087,8 +35064,8 @@
       <c r="GG135" s="58"/>
     </row>
     <row r="136" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A136" s="74"/>
-      <c r="B136" s="76"/>
+      <c r="A136" s="72"/>
+      <c r="B136" s="74"/>
       <c r="C136" s="8" t="s">
         <v>23</v>
       </c>
@@ -35280,8 +35257,8 @@
       <c r="GG136" s="58"/>
     </row>
     <row r="137" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A137" s="75"/>
-      <c r="B137" s="75"/>
+      <c r="A137" s="73"/>
+      <c r="B137" s="73"/>
       <c r="C137" s="39" t="s">
         <v>24</v>
       </c>
@@ -35473,8 +35450,8 @@
       <c r="GG137" s="58"/>
     </row>
     <row r="138" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A138" s="74"/>
-      <c r="B138" s="76"/>
+      <c r="A138" s="72"/>
+      <c r="B138" s="74"/>
       <c r="C138" s="8" t="s">
         <v>23</v>
       </c>
@@ -35666,8 +35643,8 @@
       <c r="GG138" s="58"/>
     </row>
     <row r="139" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A139" s="75"/>
-      <c r="B139" s="75"/>
+      <c r="A139" s="73"/>
+      <c r="B139" s="73"/>
       <c r="C139" s="39" t="s">
         <v>24</v>
       </c>
@@ -35859,8 +35836,8 @@
       <c r="GG139" s="58"/>
     </row>
     <row r="140" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A140" s="74"/>
-      <c r="B140" s="76"/>
+      <c r="A140" s="72"/>
+      <c r="B140" s="74"/>
       <c r="C140" s="8" t="s">
         <v>23</v>
       </c>
@@ -36052,8 +36029,8 @@
       <c r="GG140" s="58"/>
     </row>
     <row r="141" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A141" s="75"/>
-      <c r="B141" s="75"/>
+      <c r="A141" s="73"/>
+      <c r="B141" s="73"/>
       <c r="C141" s="39" t="s">
         <v>24</v>
       </c>
@@ -36245,8 +36222,8 @@
       <c r="GG141" s="58"/>
     </row>
     <row r="142" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A142" s="74"/>
-      <c r="B142" s="76"/>
+      <c r="A142" s="72"/>
+      <c r="B142" s="74"/>
       <c r="C142" s="8" t="s">
         <v>23</v>
       </c>
@@ -36438,8 +36415,8 @@
       <c r="GG142" s="58"/>
     </row>
     <row r="143" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A143" s="75"/>
-      <c r="B143" s="75"/>
+      <c r="A143" s="73"/>
+      <c r="B143" s="73"/>
       <c r="C143" s="39" t="s">
         <v>24</v>
       </c>
@@ -36631,8 +36608,8 @@
       <c r="GG143" s="58"/>
     </row>
     <row r="144" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A144" s="76"/>
-      <c r="B144" s="76"/>
+      <c r="A144" s="74"/>
+      <c r="B144" s="74"/>
       <c r="C144" s="8" t="s">
         <v>23</v>
       </c>
@@ -36824,8 +36801,8 @@
       <c r="GG144" s="59"/>
     </row>
     <row r="145" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A145" s="75"/>
-      <c r="B145" s="75"/>
+      <c r="A145" s="73"/>
+      <c r="B145" s="73"/>
       <c r="C145" s="39" t="s">
         <v>24</v>
       </c>
@@ -37017,8 +36994,8 @@
       <c r="GG145" s="59"/>
     </row>
     <row r="146" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A146" s="76"/>
-      <c r="B146" s="76"/>
+      <c r="A146" s="74"/>
+      <c r="B146" s="74"/>
       <c r="C146" s="8" t="s">
         <v>23</v>
       </c>
@@ -37210,8 +37187,8 @@
       <c r="GG146" s="59"/>
     </row>
     <row r="147" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A147" s="75"/>
-      <c r="B147" s="75"/>
+      <c r="A147" s="73"/>
+      <c r="B147" s="73"/>
       <c r="C147" s="39" t="s">
         <v>24</v>
       </c>
@@ -37403,8 +37380,8 @@
       <c r="GG147" s="59"/>
     </row>
     <row r="148" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A148" s="76"/>
-      <c r="B148" s="76"/>
+      <c r="A148" s="74"/>
+      <c r="B148" s="74"/>
       <c r="C148" s="8" t="s">
         <v>23</v>
       </c>
@@ -37596,8 +37573,8 @@
       <c r="GG148" s="59"/>
     </row>
     <row r="149" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A149" s="75"/>
-      <c r="B149" s="75"/>
+      <c r="A149" s="73"/>
+      <c r="B149" s="73"/>
       <c r="C149" s="39" t="s">
         <v>24</v>
       </c>
@@ -37789,8 +37766,8 @@
       <c r="GG149" s="59"/>
     </row>
     <row r="150" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A150" s="76"/>
-      <c r="B150" s="76"/>
+      <c r="A150" s="74"/>
+      <c r="B150" s="74"/>
       <c r="C150" s="8" t="s">
         <v>23</v>
       </c>
@@ -37982,8 +37959,8 @@
       <c r="GG150" s="59"/>
     </row>
     <row r="151" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A151" s="75"/>
-      <c r="B151" s="75"/>
+      <c r="A151" s="73"/>
+      <c r="B151" s="73"/>
       <c r="C151" s="39" t="s">
         <v>24</v>
       </c>
@@ -38175,8 +38152,8 @@
       <c r="GG151" s="59"/>
     </row>
     <row r="152" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A152" s="76"/>
-      <c r="B152" s="76"/>
+      <c r="A152" s="74"/>
+      <c r="B152" s="74"/>
       <c r="C152" s="8" t="s">
         <v>23</v>
       </c>
@@ -38368,8 +38345,8 @@
       <c r="GG152" s="59"/>
     </row>
     <row r="153" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A153" s="75"/>
-      <c r="B153" s="75"/>
+      <c r="A153" s="73"/>
+      <c r="B153" s="73"/>
       <c r="C153" s="39" t="s">
         <v>24</v>
       </c>
@@ -38561,8 +38538,8 @@
       <c r="GG153" s="59"/>
     </row>
     <row r="154" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A154" s="76"/>
-      <c r="B154" s="76"/>
+      <c r="A154" s="74"/>
+      <c r="B154" s="74"/>
       <c r="C154" s="8" t="s">
         <v>23</v>
       </c>
@@ -38754,8 +38731,8 @@
       <c r="GG154" s="59"/>
     </row>
     <row r="155" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A155" s="75"/>
-      <c r="B155" s="75"/>
+      <c r="A155" s="73"/>
+      <c r="B155" s="73"/>
       <c r="C155" s="39" t="s">
         <v>24</v>
       </c>
@@ -38947,8 +38924,8 @@
       <c r="GG155" s="59"/>
     </row>
     <row r="156" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A156" s="76"/>
-      <c r="B156" s="76"/>
+      <c r="A156" s="74"/>
+      <c r="B156" s="74"/>
       <c r="C156" s="8" t="s">
         <v>23</v>
       </c>
@@ -39140,8 +39117,8 @@
       <c r="GG156" s="59"/>
     </row>
     <row r="157" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A157" s="75"/>
-      <c r="B157" s="75"/>
+      <c r="A157" s="73"/>
+      <c r="B157" s="73"/>
       <c r="C157" s="39" t="s">
         <v>24</v>
       </c>
@@ -39333,8 +39310,8 @@
       <c r="GG157" s="59"/>
     </row>
     <row r="158" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A158" s="76"/>
-      <c r="B158" s="76"/>
+      <c r="A158" s="74"/>
+      <c r="B158" s="74"/>
       <c r="C158" s="8" t="s">
         <v>23</v>
       </c>
@@ -39526,8 +39503,8 @@
       <c r="GG158" s="59"/>
     </row>
     <row r="159" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A159" s="75"/>
-      <c r="B159" s="75"/>
+      <c r="A159" s="73"/>
+      <c r="B159" s="73"/>
       <c r="C159" s="39" t="s">
         <v>24</v>
       </c>
@@ -39719,8 +39696,8 @@
       <c r="GG159" s="59"/>
     </row>
     <row r="160" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A160" s="76"/>
-      <c r="B160" s="76"/>
+      <c r="A160" s="74"/>
+      <c r="B160" s="74"/>
       <c r="C160" s="8" t="s">
         <v>23</v>
       </c>
@@ -39912,8 +39889,8 @@
       <c r="GG160" s="59"/>
     </row>
     <row r="161" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A161" s="75"/>
-      <c r="B161" s="75"/>
+      <c r="A161" s="73"/>
+      <c r="B161" s="73"/>
       <c r="C161" s="39" t="s">
         <v>24</v>
       </c>
@@ -40105,8 +40082,8 @@
       <c r="GG161" s="59"/>
     </row>
     <row r="162" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A162" s="76"/>
-      <c r="B162" s="76"/>
+      <c r="A162" s="74"/>
+      <c r="B162" s="74"/>
       <c r="C162" s="8" t="s">
         <v>23</v>
       </c>
@@ -40298,8 +40275,8 @@
       <c r="GG162" s="59"/>
     </row>
     <row r="163" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A163" s="75"/>
-      <c r="B163" s="75"/>
+      <c r="A163" s="73"/>
+      <c r="B163" s="73"/>
       <c r="C163" s="39" t="s">
         <v>24</v>
       </c>
@@ -40491,8 +40468,8 @@
       <c r="GG163" s="59"/>
     </row>
     <row r="164" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A164" s="76"/>
-      <c r="B164" s="76"/>
+      <c r="A164" s="74"/>
+      <c r="B164" s="74"/>
       <c r="C164" s="8" t="s">
         <v>23</v>
       </c>
@@ -40684,8 +40661,8 @@
       <c r="GG164" s="59"/>
     </row>
     <row r="165" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A165" s="75"/>
-      <c r="B165" s="75"/>
+      <c r="A165" s="73"/>
+      <c r="B165" s="73"/>
       <c r="C165" s="39" t="s">
         <v>24</v>
       </c>
@@ -40877,8 +40854,8 @@
       <c r="GG165" s="59"/>
     </row>
     <row r="166" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A166" s="76"/>
-      <c r="B166" s="76"/>
+      <c r="A166" s="74"/>
+      <c r="B166" s="74"/>
       <c r="C166" s="8" t="s">
         <v>23</v>
       </c>
@@ -41070,8 +41047,8 @@
       <c r="GG166" s="59"/>
     </row>
     <row r="167" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A167" s="75"/>
-      <c r="B167" s="75"/>
+      <c r="A167" s="73"/>
+      <c r="B167" s="73"/>
       <c r="C167" s="39" t="s">
         <v>24</v>
       </c>
@@ -41263,8 +41240,8 @@
       <c r="GG167" s="59"/>
     </row>
     <row r="168" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A168" s="74"/>
-      <c r="B168" s="76"/>
+      <c r="A168" s="72"/>
+      <c r="B168" s="74"/>
       <c r="C168" s="8" t="s">
         <v>23</v>
       </c>
@@ -41456,8 +41433,8 @@
       <c r="GG168" s="59"/>
     </row>
     <row r="169" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A169" s="75"/>
-      <c r="B169" s="75"/>
+      <c r="A169" s="73"/>
+      <c r="B169" s="73"/>
       <c r="C169" s="39" t="s">
         <v>24</v>
       </c>
@@ -41649,8 +41626,8 @@
       <c r="GG169" s="59"/>
     </row>
     <row r="170" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A170" s="74"/>
-      <c r="B170" s="76"/>
+      <c r="A170" s="72"/>
+      <c r="B170" s="74"/>
       <c r="C170" s="8" t="s">
         <v>23</v>
       </c>
@@ -41842,8 +41819,8 @@
       <c r="GG170" s="59"/>
     </row>
     <row r="171" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A171" s="75"/>
-      <c r="B171" s="75"/>
+      <c r="A171" s="73"/>
+      <c r="B171" s="73"/>
       <c r="C171" s="39" t="s">
         <v>24</v>
       </c>
@@ -42035,8 +42012,8 @@
       <c r="GG171" s="59"/>
     </row>
     <row r="172" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A172" s="74"/>
-      <c r="B172" s="76"/>
+      <c r="A172" s="72"/>
+      <c r="B172" s="74"/>
       <c r="C172" s="8" t="s">
         <v>23</v>
       </c>
@@ -42228,8 +42205,8 @@
       <c r="GG172" s="59"/>
     </row>
     <row r="173" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A173" s="75"/>
-      <c r="B173" s="75"/>
+      <c r="A173" s="73"/>
+      <c r="B173" s="73"/>
       <c r="C173" s="39" t="s">
         <v>24</v>
       </c>
@@ -42421,8 +42398,8 @@
       <c r="GG173" s="59"/>
     </row>
     <row r="174" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A174" s="74"/>
-      <c r="B174" s="76"/>
+      <c r="A174" s="72"/>
+      <c r="B174" s="74"/>
       <c r="C174" s="8" t="s">
         <v>23</v>
       </c>
@@ -42614,8 +42591,8 @@
       <c r="GG174" s="59"/>
     </row>
     <row r="175" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A175" s="75"/>
-      <c r="B175" s="75"/>
+      <c r="A175" s="73"/>
+      <c r="B175" s="73"/>
       <c r="C175" s="39" t="s">
         <v>24</v>
       </c>
@@ -42807,8 +42784,8 @@
       <c r="GG175" s="59"/>
     </row>
     <row r="176" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A176" s="74"/>
-      <c r="B176" s="76"/>
+      <c r="A176" s="72"/>
+      <c r="B176" s="74"/>
       <c r="C176" s="8" t="s">
         <v>23</v>
       </c>
@@ -43000,8 +42977,8 @@
       <c r="GG176" s="59"/>
     </row>
     <row r="177" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A177" s="75"/>
-      <c r="B177" s="75"/>
+      <c r="A177" s="73"/>
+      <c r="B177" s="73"/>
       <c r="C177" s="39" t="s">
         <v>24</v>
       </c>
@@ -43193,8 +43170,8 @@
       <c r="GG177" s="59"/>
     </row>
     <row r="178" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A178" s="74"/>
-      <c r="B178" s="76"/>
+      <c r="A178" s="72"/>
+      <c r="B178" s="74"/>
       <c r="C178" s="8" t="s">
         <v>23</v>
       </c>
@@ -43386,8 +43363,8 @@
       <c r="GG178" s="59"/>
     </row>
     <row r="179" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A179" s="75"/>
-      <c r="B179" s="75"/>
+      <c r="A179" s="73"/>
+      <c r="B179" s="73"/>
       <c r="C179" s="39" t="s">
         <v>24</v>
       </c>
@@ -43579,8 +43556,8 @@
       <c r="GG179" s="59"/>
     </row>
     <row r="180" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A180" s="74"/>
-      <c r="B180" s="76"/>
+      <c r="A180" s="72"/>
+      <c r="B180" s="74"/>
       <c r="C180" s="8" t="s">
         <v>23</v>
       </c>
@@ -43772,8 +43749,8 @@
       <c r="GG180" s="59"/>
     </row>
     <row r="181" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A181" s="75"/>
-      <c r="B181" s="75"/>
+      <c r="A181" s="73"/>
+      <c r="B181" s="73"/>
       <c r="C181" s="39" t="s">
         <v>24</v>
       </c>
@@ -43965,8 +43942,8 @@
       <c r="GG181" s="59"/>
     </row>
     <row r="182" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A182" s="74"/>
-      <c r="B182" s="76"/>
+      <c r="A182" s="72"/>
+      <c r="B182" s="74"/>
       <c r="C182" s="8" t="s">
         <v>23</v>
       </c>
@@ -44158,8 +44135,8 @@
       <c r="GG182" s="59"/>
     </row>
     <row r="183" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A183" s="75"/>
-      <c r="B183" s="75"/>
+      <c r="A183" s="73"/>
+      <c r="B183" s="73"/>
       <c r="C183" s="39" t="s">
         <v>24</v>
       </c>
@@ -44351,8 +44328,8 @@
       <c r="GG183" s="59"/>
     </row>
     <row r="184" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A184" s="74"/>
-      <c r="B184" s="76"/>
+      <c r="A184" s="72"/>
+      <c r="B184" s="74"/>
       <c r="C184" s="8" t="s">
         <v>23</v>
       </c>
@@ -44544,8 +44521,8 @@
       <c r="GG184" s="59"/>
     </row>
     <row r="185" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A185" s="75"/>
-      <c r="B185" s="75"/>
+      <c r="A185" s="73"/>
+      <c r="B185" s="73"/>
       <c r="C185" s="39" t="s">
         <v>24</v>
       </c>
@@ -44737,8 +44714,8 @@
       <c r="GG185" s="59"/>
     </row>
     <row r="186" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A186" s="74"/>
-      <c r="B186" s="76"/>
+      <c r="A186" s="72"/>
+      <c r="B186" s="74"/>
       <c r="C186" s="8" t="s">
         <v>23</v>
       </c>
@@ -44930,8 +44907,8 @@
       <c r="GG186" s="59"/>
     </row>
     <row r="187" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A187" s="75"/>
-      <c r="B187" s="75"/>
+      <c r="A187" s="73"/>
+      <c r="B187" s="73"/>
       <c r="C187" s="39" t="s">
         <v>24</v>
       </c>
@@ -45123,8 +45100,8 @@
       <c r="GG187" s="59"/>
     </row>
     <row r="188" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A188" s="74"/>
-      <c r="B188" s="76"/>
+      <c r="A188" s="72"/>
+      <c r="B188" s="74"/>
       <c r="C188" s="8" t="s">
         <v>23</v>
       </c>
@@ -45316,8 +45293,8 @@
       <c r="GG188" s="59"/>
     </row>
     <row r="189" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A189" s="75"/>
-      <c r="B189" s="75"/>
+      <c r="A189" s="73"/>
+      <c r="B189" s="73"/>
       <c r="C189" s="39" t="s">
         <v>24</v>
       </c>
@@ -45509,8 +45486,8 @@
       <c r="GG189" s="59"/>
     </row>
     <row r="190" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A190" s="74"/>
-      <c r="B190" s="76"/>
+      <c r="A190" s="72"/>
+      <c r="B190" s="74"/>
       <c r="C190" s="8" t="s">
         <v>23</v>
       </c>
@@ -45702,8 +45679,8 @@
       <c r="GG190" s="59"/>
     </row>
     <row r="191" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A191" s="75"/>
-      <c r="B191" s="75"/>
+      <c r="A191" s="73"/>
+      <c r="B191" s="73"/>
       <c r="C191" s="39" t="s">
         <v>24</v>
       </c>
@@ -45895,8 +45872,8 @@
       <c r="GG191" s="59"/>
     </row>
     <row r="192" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A192" s="74"/>
-      <c r="B192" s="76"/>
+      <c r="A192" s="72"/>
+      <c r="B192" s="74"/>
       <c r="C192" s="8" t="s">
         <v>23</v>
       </c>
@@ -46088,8 +46065,8 @@
       <c r="GG192" s="59"/>
     </row>
     <row r="193" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A193" s="75"/>
-      <c r="B193" s="75"/>
+      <c r="A193" s="73"/>
+      <c r="B193" s="73"/>
       <c r="C193" s="39" t="s">
         <v>24</v>
       </c>
@@ -46281,8 +46258,8 @@
       <c r="GG193" s="59"/>
     </row>
     <row r="194" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A194" s="74"/>
-      <c r="B194" s="76"/>
+      <c r="A194" s="72"/>
+      <c r="B194" s="74"/>
       <c r="C194" s="8" t="s">
         <v>23</v>
       </c>
@@ -46474,8 +46451,8 @@
       <c r="GG194" s="59"/>
     </row>
     <row r="195" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A195" s="75"/>
-      <c r="B195" s="75"/>
+      <c r="A195" s="73"/>
+      <c r="B195" s="73"/>
       <c r="C195" s="39" t="s">
         <v>24</v>
       </c>
@@ -46667,8 +46644,8 @@
       <c r="GG195" s="59"/>
     </row>
     <row r="196" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A196" s="74"/>
-      <c r="B196" s="76"/>
+      <c r="A196" s="72"/>
+      <c r="B196" s="74"/>
       <c r="C196" s="8" t="s">
         <v>23</v>
       </c>
@@ -46860,8 +46837,8 @@
       <c r="GG196" s="59"/>
     </row>
     <row r="197" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A197" s="75"/>
-      <c r="B197" s="75"/>
+      <c r="A197" s="73"/>
+      <c r="B197" s="73"/>
       <c r="C197" s="39" t="s">
         <v>24</v>
       </c>
@@ -47053,8 +47030,8 @@
       <c r="GG197" s="59"/>
     </row>
     <row r="198" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A198" s="74"/>
-      <c r="B198" s="76"/>
+      <c r="A198" s="72"/>
+      <c r="B198" s="74"/>
       <c r="C198" s="8" t="s">
         <v>23</v>
       </c>
@@ -47246,8 +47223,8 @@
       <c r="GG198" s="59"/>
     </row>
     <row r="199" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A199" s="75"/>
-      <c r="B199" s="75"/>
+      <c r="A199" s="73"/>
+      <c r="B199" s="73"/>
       <c r="C199" s="39" t="s">
         <v>24</v>
       </c>
@@ -47439,8 +47416,8 @@
       <c r="GG199" s="59"/>
     </row>
     <row r="200" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A200" s="74"/>
-      <c r="B200" s="76"/>
+      <c r="A200" s="72"/>
+      <c r="B200" s="74"/>
       <c r="C200" s="8" t="s">
         <v>23</v>
       </c>
@@ -47632,8 +47609,8 @@
       <c r="GG200" s="59"/>
     </row>
     <row r="201" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A201" s="75"/>
-      <c r="B201" s="75"/>
+      <c r="A201" s="73"/>
+      <c r="B201" s="73"/>
       <c r="C201" s="39" t="s">
         <v>24</v>
       </c>
@@ -47825,8 +47802,8 @@
       <c r="GG201" s="59"/>
     </row>
     <row r="202" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A202" s="74"/>
-      <c r="B202" s="76"/>
+      <c r="A202" s="72"/>
+      <c r="B202" s="74"/>
       <c r="C202" s="8" t="s">
         <v>23</v>
       </c>
@@ -48018,8 +47995,8 @@
       <c r="GG202" s="59"/>
     </row>
     <row r="203" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A203" s="75"/>
-      <c r="B203" s="75"/>
+      <c r="A203" s="73"/>
+      <c r="B203" s="73"/>
       <c r="C203" s="39" t="s">
         <v>24</v>
       </c>
@@ -48211,8 +48188,8 @@
       <c r="GG203" s="59"/>
     </row>
     <row r="204" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A204" s="74"/>
-      <c r="B204" s="76"/>
+      <c r="A204" s="72"/>
+      <c r="B204" s="74"/>
       <c r="C204" s="8" t="s">
         <v>23</v>
       </c>
@@ -48404,8 +48381,8 @@
       <c r="GG204" s="59"/>
     </row>
     <row r="205" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A205" s="75"/>
-      <c r="B205" s="75"/>
+      <c r="A205" s="73"/>
+      <c r="B205" s="73"/>
       <c r="C205" s="39" t="s">
         <v>24</v>
       </c>
@@ -48597,8 +48574,8 @@
       <c r="GG205" s="59"/>
     </row>
     <row r="206" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A206" s="74"/>
-      <c r="B206" s="76"/>
+      <c r="A206" s="72"/>
+      <c r="B206" s="74"/>
       <c r="C206" s="8" t="s">
         <v>23</v>
       </c>
@@ -48790,8 +48767,8 @@
       <c r="GG206" s="59"/>
     </row>
     <row r="207" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A207" s="75"/>
-      <c r="B207" s="75"/>
+      <c r="A207" s="73"/>
+      <c r="B207" s="73"/>
       <c r="C207" s="39" t="s">
         <v>24</v>
       </c>
@@ -48983,8 +48960,8 @@
       <c r="GG207" s="59"/>
     </row>
     <row r="208" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A208" s="74"/>
-      <c r="B208" s="76"/>
+      <c r="A208" s="72"/>
+      <c r="B208" s="74"/>
       <c r="C208" s="8" t="s">
         <v>23</v>
       </c>
@@ -49176,8 +49153,8 @@
       <c r="GG208" s="59"/>
     </row>
     <row r="209" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A209" s="75"/>
-      <c r="B209" s="75"/>
+      <c r="A209" s="73"/>
+      <c r="B209" s="73"/>
       <c r="C209" s="39" t="s">
         <v>24</v>
       </c>
@@ -49369,8 +49346,8 @@
       <c r="GG209" s="59"/>
     </row>
     <row r="210" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A210" s="74"/>
-      <c r="B210" s="76"/>
+      <c r="A210" s="72"/>
+      <c r="B210" s="74"/>
       <c r="C210" s="8" t="s">
         <v>23</v>
       </c>
@@ -49562,8 +49539,8 @@
       <c r="GG210" s="59"/>
     </row>
     <row r="211" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A211" s="75"/>
-      <c r="B211" s="75"/>
+      <c r="A211" s="73"/>
+      <c r="B211" s="73"/>
       <c r="C211" s="39" t="s">
         <v>24</v>
       </c>
@@ -49755,8 +49732,8 @@
       <c r="GG211" s="59"/>
     </row>
     <row r="212" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A212" s="74"/>
-      <c r="B212" s="76"/>
+      <c r="A212" s="72"/>
+      <c r="B212" s="74"/>
       <c r="C212" s="8" t="s">
         <v>23</v>
       </c>
@@ -49948,8 +49925,8 @@
       <c r="GG212" s="59"/>
     </row>
     <row r="213" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A213" s="75"/>
-      <c r="B213" s="75"/>
+      <c r="A213" s="73"/>
+      <c r="B213" s="73"/>
       <c r="C213" s="39" t="s">
         <v>24</v>
       </c>
@@ -50141,8 +50118,8 @@
       <c r="GG213" s="59"/>
     </row>
     <row r="214" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A214" s="74"/>
-      <c r="B214" s="76"/>
+      <c r="A214" s="72"/>
+      <c r="B214" s="74"/>
       <c r="C214" s="8" t="s">
         <v>23</v>
       </c>
@@ -50334,8 +50311,8 @@
       <c r="GG214" s="59"/>
     </row>
     <row r="215" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A215" s="75"/>
-      <c r="B215" s="75"/>
+      <c r="A215" s="73"/>
+      <c r="B215" s="73"/>
       <c r="C215" s="39" t="s">
         <v>24</v>
       </c>
@@ -50527,8 +50504,8 @@
       <c r="GG215" s="59"/>
     </row>
     <row r="216" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A216" s="74"/>
-      <c r="B216" s="76"/>
+      <c r="A216" s="72"/>
+      <c r="B216" s="74"/>
       <c r="C216" s="8" t="s">
         <v>23</v>
       </c>
@@ -50720,8 +50697,8 @@
       <c r="GG216" s="59"/>
     </row>
     <row r="217" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A217" s="75"/>
-      <c r="B217" s="75"/>
+      <c r="A217" s="73"/>
+      <c r="B217" s="73"/>
       <c r="C217" s="39" t="s">
         <v>24</v>
       </c>
@@ -50913,8 +50890,8 @@
       <c r="GG217" s="59"/>
     </row>
     <row r="218" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A218" s="74"/>
-      <c r="B218" s="76"/>
+      <c r="A218" s="72"/>
+      <c r="B218" s="74"/>
       <c r="C218" s="8" t="s">
         <v>23</v>
       </c>
@@ -51106,8 +51083,8 @@
       <c r="GG218" s="59"/>
     </row>
     <row r="219" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A219" s="75"/>
-      <c r="B219" s="75"/>
+      <c r="A219" s="73"/>
+      <c r="B219" s="73"/>
       <c r="C219" s="39" t="s">
         <v>24</v>
       </c>
@@ -51299,8 +51276,8 @@
       <c r="GG219" s="59"/>
     </row>
     <row r="220" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A220" s="74"/>
-      <c r="B220" s="76"/>
+      <c r="A220" s="72"/>
+      <c r="B220" s="74"/>
       <c r="C220" s="8" t="s">
         <v>23</v>
       </c>
@@ -51492,8 +51469,8 @@
       <c r="GG220" s="59"/>
     </row>
     <row r="221" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A221" s="75"/>
-      <c r="B221" s="75"/>
+      <c r="A221" s="73"/>
+      <c r="B221" s="73"/>
       <c r="C221" s="39" t="s">
         <v>24</v>
       </c>
@@ -51685,8 +51662,8 @@
       <c r="GG221" s="59"/>
     </row>
     <row r="222" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A222" s="74"/>
-      <c r="B222" s="76"/>
+      <c r="A222" s="72"/>
+      <c r="B222" s="74"/>
       <c r="C222" s="8" t="s">
         <v>23</v>
       </c>
@@ -51878,8 +51855,8 @@
       <c r="GG222" s="59"/>
     </row>
     <row r="223" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A223" s="75"/>
-      <c r="B223" s="75"/>
+      <c r="A223" s="73"/>
+      <c r="B223" s="73"/>
       <c r="C223" s="39" t="s">
         <v>24</v>
       </c>
@@ -52071,8 +52048,8 @@
       <c r="GG223" s="59"/>
     </row>
     <row r="224" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A224" s="74"/>
-      <c r="B224" s="76"/>
+      <c r="A224" s="72"/>
+      <c r="B224" s="74"/>
       <c r="C224" s="8" t="s">
         <v>23</v>
       </c>
@@ -52264,8 +52241,8 @@
       <c r="GG224" s="59"/>
     </row>
     <row r="225" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A225" s="75"/>
-      <c r="B225" s="75"/>
+      <c r="A225" s="73"/>
+      <c r="B225" s="73"/>
       <c r="C225" s="39" t="s">
         <v>24</v>
       </c>
@@ -52457,8 +52434,8 @@
       <c r="GG225" s="59"/>
     </row>
     <row r="226" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A226" s="74"/>
-      <c r="B226" s="76"/>
+      <c r="A226" s="72"/>
+      <c r="B226" s="74"/>
       <c r="C226" s="8" t="s">
         <v>23</v>
       </c>
@@ -52650,8 +52627,8 @@
       <c r="GG226" s="59"/>
     </row>
     <row r="227" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A227" s="75"/>
-      <c r="B227" s="75"/>
+      <c r="A227" s="73"/>
+      <c r="B227" s="73"/>
       <c r="C227" s="39" t="s">
         <v>24</v>
       </c>
@@ -52843,8 +52820,8 @@
       <c r="GG227" s="59"/>
     </row>
     <row r="228" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A228" s="74"/>
-      <c r="B228" s="76"/>
+      <c r="A228" s="72"/>
+      <c r="B228" s="74"/>
       <c r="C228" s="8" t="s">
         <v>23</v>
       </c>
@@ -53036,8 +53013,8 @@
       <c r="GG228" s="59"/>
     </row>
     <row r="229" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A229" s="75"/>
-      <c r="B229" s="75"/>
+      <c r="A229" s="73"/>
+      <c r="B229" s="73"/>
       <c r="C229" s="39" t="s">
         <v>24</v>
       </c>
@@ -53229,8 +53206,8 @@
       <c r="GG229" s="59"/>
     </row>
     <row r="230" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A230" s="74"/>
-      <c r="B230" s="76"/>
+      <c r="A230" s="72"/>
+      <c r="B230" s="74"/>
       <c r="C230" s="8" t="s">
         <v>23</v>
       </c>
@@ -53422,8 +53399,8 @@
       <c r="GG230" s="59"/>
     </row>
     <row r="231" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A231" s="75"/>
-      <c r="B231" s="75"/>
+      <c r="A231" s="73"/>
+      <c r="B231" s="73"/>
       <c r="C231" s="39" t="s">
         <v>24</v>
       </c>
@@ -53615,8 +53592,8 @@
       <c r="GG231" s="59"/>
     </row>
     <row r="232" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A232" s="74"/>
-      <c r="B232" s="76"/>
+      <c r="A232" s="72"/>
+      <c r="B232" s="74"/>
       <c r="C232" s="8" t="s">
         <v>23</v>
       </c>
@@ -53808,8 +53785,8 @@
       <c r="GG232" s="59"/>
     </row>
     <row r="233" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A233" s="75"/>
-      <c r="B233" s="75"/>
+      <c r="A233" s="73"/>
+      <c r="B233" s="73"/>
       <c r="C233" s="39" t="s">
         <v>24</v>
       </c>
@@ -54001,8 +53978,8 @@
       <c r="GG233" s="59"/>
     </row>
     <row r="234" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A234" s="74"/>
-      <c r="B234" s="76"/>
+      <c r="A234" s="72"/>
+      <c r="B234" s="74"/>
       <c r="C234" s="8" t="s">
         <v>23</v>
       </c>
@@ -54194,8 +54171,8 @@
       <c r="GG234" s="59"/>
     </row>
     <row r="235" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A235" s="75"/>
-      <c r="B235" s="75"/>
+      <c r="A235" s="73"/>
+      <c r="B235" s="73"/>
       <c r="C235" s="39" t="s">
         <v>24</v>
       </c>
@@ -54387,8 +54364,8 @@
       <c r="GG235" s="59"/>
     </row>
     <row r="236" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A236" s="74"/>
-      <c r="B236" s="76"/>
+      <c r="A236" s="72"/>
+      <c r="B236" s="74"/>
       <c r="C236" s="8" t="s">
         <v>23</v>
       </c>
@@ -54580,8 +54557,8 @@
       <c r="GG236" s="59"/>
     </row>
     <row r="237" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A237" s="75"/>
-      <c r="B237" s="75"/>
+      <c r="A237" s="73"/>
+      <c r="B237" s="73"/>
       <c r="C237" s="39" t="s">
         <v>24</v>
       </c>
@@ -54773,8 +54750,8 @@
       <c r="GG237" s="59"/>
     </row>
     <row r="238" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A238" s="74"/>
-      <c r="B238" s="76"/>
+      <c r="A238" s="72"/>
+      <c r="B238" s="74"/>
       <c r="C238" s="8" t="s">
         <v>23</v>
       </c>
@@ -54966,8 +54943,8 @@
       <c r="GG238" s="59"/>
     </row>
     <row r="239" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A239" s="75"/>
-      <c r="B239" s="75"/>
+      <c r="A239" s="73"/>
+      <c r="B239" s="73"/>
       <c r="C239" s="39" t="s">
         <v>24</v>
       </c>
@@ -55159,8 +55136,8 @@
       <c r="GG239" s="59"/>
     </row>
     <row r="240" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A240" s="74"/>
-      <c r="B240" s="76"/>
+      <c r="A240" s="72"/>
+      <c r="B240" s="74"/>
       <c r="C240" s="8" t="s">
         <v>23</v>
       </c>
@@ -55352,8 +55329,8 @@
       <c r="GG240" s="59"/>
     </row>
     <row r="241" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A241" s="75"/>
-      <c r="B241" s="75"/>
+      <c r="A241" s="73"/>
+      <c r="B241" s="73"/>
       <c r="C241" s="39" t="s">
         <v>24</v>
       </c>
@@ -55545,8 +55522,8 @@
       <c r="GG241" s="59"/>
     </row>
     <row r="242" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A242" s="74"/>
-      <c r="B242" s="76"/>
+      <c r="A242" s="72"/>
+      <c r="B242" s="74"/>
       <c r="C242" s="8" t="s">
         <v>23</v>
       </c>
@@ -55738,8 +55715,8 @@
       <c r="GG242" s="59"/>
     </row>
     <row r="243" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A243" s="75"/>
-      <c r="B243" s="75"/>
+      <c r="A243" s="73"/>
+      <c r="B243" s="73"/>
       <c r="C243" s="39" t="s">
         <v>24</v>
       </c>
@@ -55931,8 +55908,8 @@
       <c r="GG243" s="59"/>
     </row>
     <row r="244" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A244" s="74"/>
-      <c r="B244" s="76"/>
+      <c r="A244" s="72"/>
+      <c r="B244" s="74"/>
       <c r="C244" s="8" t="s">
         <v>23</v>
       </c>
@@ -56124,8 +56101,8 @@
       <c r="GG244" s="59"/>
     </row>
     <row r="245" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A245" s="75"/>
-      <c r="B245" s="75"/>
+      <c r="A245" s="73"/>
+      <c r="B245" s="73"/>
       <c r="C245" s="39" t="s">
         <v>24</v>
       </c>
@@ -56317,8 +56294,8 @@
       <c r="GG245" s="59"/>
     </row>
     <row r="246" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A246" s="74"/>
-      <c r="B246" s="76"/>
+      <c r="A246" s="72"/>
+      <c r="B246" s="74"/>
       <c r="C246" s="8" t="s">
         <v>23</v>
       </c>
@@ -56510,8 +56487,8 @@
       <c r="GG246" s="59"/>
     </row>
     <row r="247" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A247" s="75"/>
-      <c r="B247" s="75"/>
+      <c r="A247" s="73"/>
+      <c r="B247" s="73"/>
       <c r="C247" s="39" t="s">
         <v>24</v>
       </c>
@@ -56703,8 +56680,8 @@
       <c r="GG247" s="59"/>
     </row>
     <row r="248" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A248" s="74"/>
-      <c r="B248" s="76"/>
+      <c r="A248" s="72"/>
+      <c r="B248" s="74"/>
       <c r="C248" s="8" t="s">
         <v>23</v>
       </c>
@@ -56896,8 +56873,8 @@
       <c r="GG248" s="59"/>
     </row>
     <row r="249" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A249" s="75"/>
-      <c r="B249" s="75"/>
+      <c r="A249" s="73"/>
+      <c r="B249" s="73"/>
       <c r="C249" s="39" t="s">
         <v>24</v>
       </c>
@@ -57089,8 +57066,8 @@
       <c r="GG249" s="59"/>
     </row>
     <row r="250" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A250" s="74"/>
-      <c r="B250" s="76"/>
+      <c r="A250" s="72"/>
+      <c r="B250" s="74"/>
       <c r="C250" s="8" t="s">
         <v>23</v>
       </c>
@@ -57282,8 +57259,8 @@
       <c r="GG250" s="59"/>
     </row>
     <row r="251" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A251" s="75"/>
-      <c r="B251" s="75"/>
+      <c r="A251" s="73"/>
+      <c r="B251" s="73"/>
       <c r="C251" s="39" t="s">
         <v>24</v>
       </c>
@@ -57475,8 +57452,8 @@
       <c r="GG251" s="59"/>
     </row>
     <row r="252" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A252" s="74"/>
-      <c r="B252" s="76"/>
+      <c r="A252" s="72"/>
+      <c r="B252" s="74"/>
       <c r="C252" s="8" t="s">
         <v>23</v>
       </c>
@@ -57668,8 +57645,8 @@
       <c r="GG252" s="59"/>
     </row>
     <row r="253" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A253" s="75"/>
-      <c r="B253" s="75"/>
+      <c r="A253" s="73"/>
+      <c r="B253" s="73"/>
       <c r="C253" s="39" t="s">
         <v>24</v>
       </c>
@@ -57861,8 +57838,8 @@
       <c r="GG253" s="59"/>
     </row>
     <row r="254" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A254" s="74"/>
-      <c r="B254" s="76"/>
+      <c r="A254" s="72"/>
+      <c r="B254" s="74"/>
       <c r="C254" s="8" t="s">
         <v>23</v>
       </c>
@@ -58054,8 +58031,8 @@
       <c r="GG254" s="59"/>
     </row>
     <row r="255" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A255" s="75"/>
-      <c r="B255" s="75"/>
+      <c r="A255" s="73"/>
+      <c r="B255" s="73"/>
       <c r="C255" s="39" t="s">
         <v>24</v>
       </c>
@@ -58247,8 +58224,8 @@
       <c r="GG255" s="59"/>
     </row>
     <row r="256" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A256" s="74"/>
-      <c r="B256" s="76"/>
+      <c r="A256" s="72"/>
+      <c r="B256" s="74"/>
       <c r="C256" s="8" t="s">
         <v>23</v>
       </c>
@@ -58440,8 +58417,8 @@
       <c r="GG256" s="59"/>
     </row>
     <row r="257" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A257" s="75"/>
-      <c r="B257" s="75"/>
+      <c r="A257" s="73"/>
+      <c r="B257" s="73"/>
       <c r="C257" s="39" t="s">
         <v>24</v>
       </c>
@@ -58633,8 +58610,8 @@
       <c r="GG257" s="59"/>
     </row>
     <row r="258" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A258" s="74"/>
-      <c r="B258" s="76"/>
+      <c r="A258" s="72"/>
+      <c r="B258" s="74"/>
       <c r="C258" s="8" t="s">
         <v>23</v>
       </c>
@@ -58826,8 +58803,8 @@
       <c r="GG258" s="59"/>
     </row>
     <row r="259" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A259" s="75"/>
-      <c r="B259" s="75"/>
+      <c r="A259" s="73"/>
+      <c r="B259" s="73"/>
       <c r="C259" s="39" t="s">
         <v>24</v>
       </c>
@@ -59019,8 +58996,8 @@
       <c r="GG259" s="59"/>
     </row>
     <row r="260" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A260" s="74"/>
-      <c r="B260" s="76"/>
+      <c r="A260" s="72"/>
+      <c r="B260" s="74"/>
       <c r="C260" s="8" t="s">
         <v>23</v>
       </c>
@@ -59212,8 +59189,8 @@
       <c r="GG260" s="59"/>
     </row>
     <row r="261" spans="1:189" x14ac:dyDescent="0.25">
-      <c r="A261" s="75"/>
-      <c r="B261" s="75"/>
+      <c r="A261" s="73"/>
+      <c r="B261" s="73"/>
       <c r="C261" s="39" t="s">
         <v>24</v>
       </c>
@@ -61662,6 +61639,386 @@
     </row>
   </sheetData>
   <mergeCells count="404">
+    <mergeCell ref="JK11:JM11"/>
+    <mergeCell ref="JN11:JP11"/>
+    <mergeCell ref="JQ11:JS11"/>
+    <mergeCell ref="JT11:JV11"/>
+    <mergeCell ref="JW11:JY11"/>
+    <mergeCell ref="JZ11:KB11"/>
+    <mergeCell ref="KC11:KE11"/>
+    <mergeCell ref="IJ11:IL11"/>
+    <mergeCell ref="IM11:IO11"/>
+    <mergeCell ref="IP11:IR11"/>
+    <mergeCell ref="IS11:IU11"/>
+    <mergeCell ref="IV11:IX11"/>
+    <mergeCell ref="IY11:JA11"/>
+    <mergeCell ref="JB11:JD11"/>
+    <mergeCell ref="JE11:JG11"/>
+    <mergeCell ref="JH11:JJ11"/>
+    <mergeCell ref="HI11:HK11"/>
+    <mergeCell ref="HL11:HN11"/>
+    <mergeCell ref="HO11:HQ11"/>
+    <mergeCell ref="HR11:HT11"/>
+    <mergeCell ref="HU11:HW11"/>
+    <mergeCell ref="HX11:HZ11"/>
+    <mergeCell ref="IA11:IC11"/>
+    <mergeCell ref="ID11:IF11"/>
+    <mergeCell ref="IG11:II11"/>
+    <mergeCell ref="GH11:GJ11"/>
+    <mergeCell ref="GK11:GM11"/>
+    <mergeCell ref="GN11:GP11"/>
+    <mergeCell ref="GQ11:GS11"/>
+    <mergeCell ref="GT11:GV11"/>
+    <mergeCell ref="GW11:GY11"/>
+    <mergeCell ref="GZ11:HB11"/>
+    <mergeCell ref="HC11:HE11"/>
+    <mergeCell ref="HF11:HH11"/>
+    <mergeCell ref="A140:A141"/>
+    <mergeCell ref="B140:B141"/>
+    <mergeCell ref="A142:A143"/>
+    <mergeCell ref="B142:B143"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="B134:B135"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="B136:B137"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="B138:B139"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="B120:B121"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="A124:A125"/>
+    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="A126:A127"/>
+    <mergeCell ref="B126:B127"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="B128:B129"/>
+    <mergeCell ref="A110:A111"/>
+    <mergeCell ref="B110:B111"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="B112:B113"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="B116:B117"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="B100:B101"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="B102:B103"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="B106:B107"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="B108:B109"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="FS24:FU24"/>
+    <mergeCell ref="FV24:FX24"/>
+    <mergeCell ref="FY24:GA24"/>
+    <mergeCell ref="GB24:GD24"/>
+    <mergeCell ref="GE24:GG24"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="ER24:ET24"/>
+    <mergeCell ref="EU24:EW24"/>
+    <mergeCell ref="EX24:EZ24"/>
+    <mergeCell ref="FA24:FC24"/>
+    <mergeCell ref="FD24:FF24"/>
+    <mergeCell ref="FG24:FI24"/>
+    <mergeCell ref="FJ24:FL24"/>
+    <mergeCell ref="FM24:FO24"/>
+    <mergeCell ref="FP24:FR24"/>
+    <mergeCell ref="DQ24:DS24"/>
+    <mergeCell ref="DT24:DV24"/>
+    <mergeCell ref="DW24:DY24"/>
+    <mergeCell ref="DZ24:EB24"/>
+    <mergeCell ref="EC24:EE24"/>
+    <mergeCell ref="EF24:EH24"/>
+    <mergeCell ref="CD24:CF24"/>
+    <mergeCell ref="CG24:CI24"/>
+    <mergeCell ref="CJ24:CL24"/>
+    <mergeCell ref="CM24:CO24"/>
+    <mergeCell ref="EI24:EK24"/>
+    <mergeCell ref="EL24:EN24"/>
+    <mergeCell ref="EO24:EQ24"/>
+    <mergeCell ref="CP24:CR24"/>
+    <mergeCell ref="CS24:CU24"/>
+    <mergeCell ref="CV24:CX24"/>
+    <mergeCell ref="CY24:DA24"/>
+    <mergeCell ref="DB24:DD24"/>
+    <mergeCell ref="DE24:DG24"/>
+    <mergeCell ref="DH24:DJ24"/>
+    <mergeCell ref="DK24:DM24"/>
+    <mergeCell ref="DN24:DP24"/>
+    <mergeCell ref="BC24:BE24"/>
+    <mergeCell ref="BF24:BH24"/>
+    <mergeCell ref="BI24:BK24"/>
+    <mergeCell ref="BL24:BN24"/>
+    <mergeCell ref="BO24:BQ24"/>
+    <mergeCell ref="BR24:BT24"/>
+    <mergeCell ref="BU24:BW24"/>
+    <mergeCell ref="BX24:BZ24"/>
+    <mergeCell ref="CA24:CC24"/>
+    <mergeCell ref="BF11:BH11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="D4:J4"/>
+    <mergeCell ref="D5:J5"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="V24:X24"/>
+    <mergeCell ref="Y24:AA24"/>
+    <mergeCell ref="AB24:AD24"/>
+    <mergeCell ref="AE24:AG24"/>
+    <mergeCell ref="AH24:AJ24"/>
+    <mergeCell ref="AK24:AM24"/>
+    <mergeCell ref="AN24:AP24"/>
+    <mergeCell ref="AQ24:AS24"/>
+    <mergeCell ref="AT24:AV24"/>
+    <mergeCell ref="AW24:AY24"/>
+    <mergeCell ref="AZ24:BB24"/>
+    <mergeCell ref="AE11:AG11"/>
+    <mergeCell ref="AH11:AJ11"/>
+    <mergeCell ref="AK11:AM11"/>
+    <mergeCell ref="AN11:AP11"/>
+    <mergeCell ref="AQ11:AS11"/>
+    <mergeCell ref="AT11:AV11"/>
+    <mergeCell ref="AW11:AY11"/>
+    <mergeCell ref="AZ11:BB11"/>
+    <mergeCell ref="BC11:BE11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="S11:U11"/>
+    <mergeCell ref="V11:X11"/>
+    <mergeCell ref="Y11:AA11"/>
+    <mergeCell ref="AB11:AD11"/>
+    <mergeCell ref="BI11:BK11"/>
+    <mergeCell ref="BL11:BN11"/>
+    <mergeCell ref="BO11:BQ11"/>
+    <mergeCell ref="BR11:BT11"/>
+    <mergeCell ref="BU11:BW11"/>
+    <mergeCell ref="BX11:BZ11"/>
+    <mergeCell ref="CA11:CC11"/>
+    <mergeCell ref="CD11:CF11"/>
+    <mergeCell ref="CG11:CI11"/>
+    <mergeCell ref="EC11:EE11"/>
+    <mergeCell ref="EF11:EH11"/>
+    <mergeCell ref="EI11:EK11"/>
+    <mergeCell ref="CJ11:CL11"/>
+    <mergeCell ref="CM11:CO11"/>
+    <mergeCell ref="CP11:CR11"/>
+    <mergeCell ref="CS11:CU11"/>
+    <mergeCell ref="CV11:CX11"/>
+    <mergeCell ref="CY11:DA11"/>
+    <mergeCell ref="DB11:DD11"/>
+    <mergeCell ref="DE11:DG11"/>
+    <mergeCell ref="DH11:DJ11"/>
+    <mergeCell ref="FM11:FO11"/>
+    <mergeCell ref="FP11:FR11"/>
+    <mergeCell ref="FS11:FU11"/>
+    <mergeCell ref="FV11:FX11"/>
+    <mergeCell ref="FY11:GA11"/>
+    <mergeCell ref="GB11:GD11"/>
+    <mergeCell ref="GE11:GG11"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="EL11:EN11"/>
+    <mergeCell ref="EO11:EQ11"/>
+    <mergeCell ref="ER11:ET11"/>
+    <mergeCell ref="EU11:EW11"/>
+    <mergeCell ref="EX11:EZ11"/>
+    <mergeCell ref="FA11:FC11"/>
+    <mergeCell ref="FD11:FF11"/>
+    <mergeCell ref="FG11:FI11"/>
+    <mergeCell ref="FJ11:FL11"/>
+    <mergeCell ref="DK11:DM11"/>
+    <mergeCell ref="DN11:DP11"/>
+    <mergeCell ref="DQ11:DS11"/>
+    <mergeCell ref="DT11:DV11"/>
+    <mergeCell ref="DW11:DY11"/>
+    <mergeCell ref="DZ11:EB11"/>
+    <mergeCell ref="A144:A145"/>
+    <mergeCell ref="B144:B145"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="B146:B147"/>
+    <mergeCell ref="A148:A149"/>
+    <mergeCell ref="B148:B149"/>
+    <mergeCell ref="A150:A151"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="A152:A153"/>
+    <mergeCell ref="B152:B153"/>
+    <mergeCell ref="A154:A155"/>
+    <mergeCell ref="B154:B155"/>
+    <mergeCell ref="A156:A157"/>
+    <mergeCell ref="B156:B157"/>
+    <mergeCell ref="A158:A159"/>
+    <mergeCell ref="B158:B159"/>
+    <mergeCell ref="A160:A161"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="A162:A163"/>
+    <mergeCell ref="B162:B163"/>
+    <mergeCell ref="A164:A165"/>
+    <mergeCell ref="B164:B165"/>
+    <mergeCell ref="A166:A167"/>
+    <mergeCell ref="B166:B167"/>
+    <mergeCell ref="A168:A169"/>
+    <mergeCell ref="B168:B169"/>
+    <mergeCell ref="A170:A171"/>
+    <mergeCell ref="B170:B171"/>
+    <mergeCell ref="A172:A173"/>
+    <mergeCell ref="B172:B173"/>
+    <mergeCell ref="A174:A175"/>
+    <mergeCell ref="B174:B175"/>
+    <mergeCell ref="A176:A177"/>
+    <mergeCell ref="B176:B177"/>
+    <mergeCell ref="A178:A179"/>
+    <mergeCell ref="B178:B179"/>
+    <mergeCell ref="A180:A181"/>
+    <mergeCell ref="B180:B181"/>
+    <mergeCell ref="A182:A183"/>
+    <mergeCell ref="B182:B183"/>
+    <mergeCell ref="A184:A185"/>
+    <mergeCell ref="B184:B185"/>
+    <mergeCell ref="A186:A187"/>
+    <mergeCell ref="B186:B187"/>
+    <mergeCell ref="A188:A189"/>
+    <mergeCell ref="B188:B189"/>
+    <mergeCell ref="A190:A191"/>
+    <mergeCell ref="B190:B191"/>
+    <mergeCell ref="A192:A193"/>
+    <mergeCell ref="B192:B193"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="B194:B195"/>
+    <mergeCell ref="A196:A197"/>
+    <mergeCell ref="B196:B197"/>
+    <mergeCell ref="A198:A199"/>
+    <mergeCell ref="B198:B199"/>
+    <mergeCell ref="A200:A201"/>
+    <mergeCell ref="B200:B201"/>
+    <mergeCell ref="A202:A203"/>
+    <mergeCell ref="B202:B203"/>
+    <mergeCell ref="A204:A205"/>
+    <mergeCell ref="B204:B205"/>
+    <mergeCell ref="A206:A207"/>
+    <mergeCell ref="B206:B207"/>
+    <mergeCell ref="A208:A209"/>
+    <mergeCell ref="B208:B209"/>
+    <mergeCell ref="A210:A211"/>
+    <mergeCell ref="B210:B211"/>
+    <mergeCell ref="A212:A213"/>
+    <mergeCell ref="B212:B213"/>
+    <mergeCell ref="A214:A215"/>
+    <mergeCell ref="B214:B215"/>
+    <mergeCell ref="A216:A217"/>
+    <mergeCell ref="B216:B217"/>
+    <mergeCell ref="A218:A219"/>
+    <mergeCell ref="B218:B219"/>
+    <mergeCell ref="A220:A221"/>
+    <mergeCell ref="B220:B221"/>
+    <mergeCell ref="A222:A223"/>
+    <mergeCell ref="B222:B223"/>
+    <mergeCell ref="A238:A239"/>
+    <mergeCell ref="B238:B239"/>
+    <mergeCell ref="A240:A241"/>
+    <mergeCell ref="B240:B241"/>
+    <mergeCell ref="A242:A243"/>
+    <mergeCell ref="B242:B243"/>
+    <mergeCell ref="A224:A225"/>
+    <mergeCell ref="B224:B225"/>
+    <mergeCell ref="A226:A227"/>
+    <mergeCell ref="B226:B227"/>
+    <mergeCell ref="A228:A229"/>
+    <mergeCell ref="B228:B229"/>
+    <mergeCell ref="A230:A231"/>
+    <mergeCell ref="B230:B231"/>
+    <mergeCell ref="A232:A233"/>
+    <mergeCell ref="B232:B233"/>
     <mergeCell ref="A254:A255"/>
     <mergeCell ref="B254:B255"/>
     <mergeCell ref="A256:A257"/>
@@ -61686,386 +62043,6 @@
     <mergeCell ref="B234:B235"/>
     <mergeCell ref="A236:A237"/>
     <mergeCell ref="B236:B237"/>
-    <mergeCell ref="A238:A239"/>
-    <mergeCell ref="B238:B239"/>
-    <mergeCell ref="A240:A241"/>
-    <mergeCell ref="B240:B241"/>
-    <mergeCell ref="A242:A243"/>
-    <mergeCell ref="B242:B243"/>
-    <mergeCell ref="A224:A225"/>
-    <mergeCell ref="B224:B225"/>
-    <mergeCell ref="A226:A227"/>
-    <mergeCell ref="B226:B227"/>
-    <mergeCell ref="A228:A229"/>
-    <mergeCell ref="B228:B229"/>
-    <mergeCell ref="A230:A231"/>
-    <mergeCell ref="B230:B231"/>
-    <mergeCell ref="A232:A233"/>
-    <mergeCell ref="B232:B233"/>
-    <mergeCell ref="A214:A215"/>
-    <mergeCell ref="B214:B215"/>
-    <mergeCell ref="A216:A217"/>
-    <mergeCell ref="B216:B217"/>
-    <mergeCell ref="A218:A219"/>
-    <mergeCell ref="B218:B219"/>
-    <mergeCell ref="A220:A221"/>
-    <mergeCell ref="B220:B221"/>
-    <mergeCell ref="A222:A223"/>
-    <mergeCell ref="B222:B223"/>
-    <mergeCell ref="A204:A205"/>
-    <mergeCell ref="B204:B205"/>
-    <mergeCell ref="A206:A207"/>
-    <mergeCell ref="B206:B207"/>
-    <mergeCell ref="A208:A209"/>
-    <mergeCell ref="B208:B209"/>
-    <mergeCell ref="A210:A211"/>
-    <mergeCell ref="B210:B211"/>
-    <mergeCell ref="A212:A213"/>
-    <mergeCell ref="B212:B213"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="B194:B195"/>
-    <mergeCell ref="A196:A197"/>
-    <mergeCell ref="B196:B197"/>
-    <mergeCell ref="A198:A199"/>
-    <mergeCell ref="B198:B199"/>
-    <mergeCell ref="A200:A201"/>
-    <mergeCell ref="B200:B201"/>
-    <mergeCell ref="A202:A203"/>
-    <mergeCell ref="B202:B203"/>
-    <mergeCell ref="A184:A185"/>
-    <mergeCell ref="B184:B185"/>
-    <mergeCell ref="A186:A187"/>
-    <mergeCell ref="B186:B187"/>
-    <mergeCell ref="A188:A189"/>
-    <mergeCell ref="B188:B189"/>
-    <mergeCell ref="A190:A191"/>
-    <mergeCell ref="B190:B191"/>
-    <mergeCell ref="A192:A193"/>
-    <mergeCell ref="B192:B193"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="B174:B175"/>
-    <mergeCell ref="A176:A177"/>
-    <mergeCell ref="B176:B177"/>
-    <mergeCell ref="A178:A179"/>
-    <mergeCell ref="B178:B179"/>
-    <mergeCell ref="A180:A181"/>
-    <mergeCell ref="B180:B181"/>
-    <mergeCell ref="A182:A183"/>
-    <mergeCell ref="B182:B183"/>
-    <mergeCell ref="A164:A165"/>
-    <mergeCell ref="B164:B165"/>
-    <mergeCell ref="A166:A167"/>
-    <mergeCell ref="B166:B167"/>
-    <mergeCell ref="A168:A169"/>
-    <mergeCell ref="B168:B169"/>
-    <mergeCell ref="A170:A171"/>
-    <mergeCell ref="B170:B171"/>
-    <mergeCell ref="A172:A173"/>
-    <mergeCell ref="B172:B173"/>
-    <mergeCell ref="A154:A155"/>
-    <mergeCell ref="B154:B155"/>
-    <mergeCell ref="A156:A157"/>
-    <mergeCell ref="B156:B157"/>
-    <mergeCell ref="A158:A159"/>
-    <mergeCell ref="B158:B159"/>
-    <mergeCell ref="A160:A161"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="A162:A163"/>
-    <mergeCell ref="B162:B163"/>
-    <mergeCell ref="A144:A145"/>
-    <mergeCell ref="B144:B145"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="B146:B147"/>
-    <mergeCell ref="A148:A149"/>
-    <mergeCell ref="B148:B149"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="B150:B151"/>
-    <mergeCell ref="A152:A153"/>
-    <mergeCell ref="B152:B153"/>
-    <mergeCell ref="FM11:FO11"/>
-    <mergeCell ref="FP11:FR11"/>
-    <mergeCell ref="FS11:FU11"/>
-    <mergeCell ref="FV11:FX11"/>
-    <mergeCell ref="FY11:GA11"/>
-    <mergeCell ref="GB11:GD11"/>
-    <mergeCell ref="GE11:GG11"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="EL11:EN11"/>
-    <mergeCell ref="EO11:EQ11"/>
-    <mergeCell ref="ER11:ET11"/>
-    <mergeCell ref="EU11:EW11"/>
-    <mergeCell ref="EX11:EZ11"/>
-    <mergeCell ref="FA11:FC11"/>
-    <mergeCell ref="FD11:FF11"/>
-    <mergeCell ref="FG11:FI11"/>
-    <mergeCell ref="FJ11:FL11"/>
-    <mergeCell ref="DK11:DM11"/>
-    <mergeCell ref="DN11:DP11"/>
-    <mergeCell ref="DQ11:DS11"/>
-    <mergeCell ref="DT11:DV11"/>
-    <mergeCell ref="DW11:DY11"/>
-    <mergeCell ref="DZ11:EB11"/>
-    <mergeCell ref="EC11:EE11"/>
-    <mergeCell ref="EF11:EH11"/>
-    <mergeCell ref="EI11:EK11"/>
-    <mergeCell ref="CJ11:CL11"/>
-    <mergeCell ref="CM11:CO11"/>
-    <mergeCell ref="CP11:CR11"/>
-    <mergeCell ref="CS11:CU11"/>
-    <mergeCell ref="CV11:CX11"/>
-    <mergeCell ref="CY11:DA11"/>
-    <mergeCell ref="DB11:DD11"/>
-    <mergeCell ref="DE11:DG11"/>
-    <mergeCell ref="DH11:DJ11"/>
-    <mergeCell ref="BI11:BK11"/>
-    <mergeCell ref="BL11:BN11"/>
-    <mergeCell ref="BO11:BQ11"/>
-    <mergeCell ref="BR11:BT11"/>
-    <mergeCell ref="BU11:BW11"/>
-    <mergeCell ref="BX11:BZ11"/>
-    <mergeCell ref="CA11:CC11"/>
-    <mergeCell ref="CD11:CF11"/>
-    <mergeCell ref="CG11:CI11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="S11:U11"/>
-    <mergeCell ref="V11:X11"/>
-    <mergeCell ref="Y11:AA11"/>
-    <mergeCell ref="AB11:AD11"/>
-    <mergeCell ref="AE11:AG11"/>
-    <mergeCell ref="AH11:AJ11"/>
-    <mergeCell ref="AK11:AM11"/>
-    <mergeCell ref="AN11:AP11"/>
-    <mergeCell ref="AQ11:AS11"/>
-    <mergeCell ref="AT11:AV11"/>
-    <mergeCell ref="AW11:AY11"/>
-    <mergeCell ref="AZ11:BB11"/>
-    <mergeCell ref="BC11:BE11"/>
-    <mergeCell ref="BF11:BH11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="D3:J3"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="V24:X24"/>
-    <mergeCell ref="Y24:AA24"/>
-    <mergeCell ref="AB24:AD24"/>
-    <mergeCell ref="AE24:AG24"/>
-    <mergeCell ref="AH24:AJ24"/>
-    <mergeCell ref="AK24:AM24"/>
-    <mergeCell ref="AN24:AP24"/>
-    <mergeCell ref="AQ24:AS24"/>
-    <mergeCell ref="AT24:AV24"/>
-    <mergeCell ref="AW24:AY24"/>
-    <mergeCell ref="AZ24:BB24"/>
-    <mergeCell ref="BC24:BE24"/>
-    <mergeCell ref="BF24:BH24"/>
-    <mergeCell ref="BI24:BK24"/>
-    <mergeCell ref="BL24:BN24"/>
-    <mergeCell ref="BO24:BQ24"/>
-    <mergeCell ref="BR24:BT24"/>
-    <mergeCell ref="BU24:BW24"/>
-    <mergeCell ref="BX24:BZ24"/>
-    <mergeCell ref="CA24:CC24"/>
-    <mergeCell ref="CD24:CF24"/>
-    <mergeCell ref="CG24:CI24"/>
-    <mergeCell ref="CJ24:CL24"/>
-    <mergeCell ref="CM24:CO24"/>
-    <mergeCell ref="EI24:EK24"/>
-    <mergeCell ref="EL24:EN24"/>
-    <mergeCell ref="EO24:EQ24"/>
-    <mergeCell ref="CP24:CR24"/>
-    <mergeCell ref="CS24:CU24"/>
-    <mergeCell ref="CV24:CX24"/>
-    <mergeCell ref="CY24:DA24"/>
-    <mergeCell ref="DB24:DD24"/>
-    <mergeCell ref="DE24:DG24"/>
-    <mergeCell ref="DH24:DJ24"/>
-    <mergeCell ref="DK24:DM24"/>
-    <mergeCell ref="DN24:DP24"/>
-    <mergeCell ref="FS24:FU24"/>
-    <mergeCell ref="FV24:FX24"/>
-    <mergeCell ref="FY24:GA24"/>
-    <mergeCell ref="GB24:GD24"/>
-    <mergeCell ref="GE24:GG24"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="ER24:ET24"/>
-    <mergeCell ref="EU24:EW24"/>
-    <mergeCell ref="EX24:EZ24"/>
-    <mergeCell ref="FA24:FC24"/>
-    <mergeCell ref="FD24:FF24"/>
-    <mergeCell ref="FG24:FI24"/>
-    <mergeCell ref="FJ24:FL24"/>
-    <mergeCell ref="FM24:FO24"/>
-    <mergeCell ref="FP24:FR24"/>
-    <mergeCell ref="DQ24:DS24"/>
-    <mergeCell ref="DT24:DV24"/>
-    <mergeCell ref="DW24:DY24"/>
-    <mergeCell ref="DZ24:EB24"/>
-    <mergeCell ref="EC24:EE24"/>
-    <mergeCell ref="EF24:EH24"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="B100:B101"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="B102:B103"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="B104:B105"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="B106:B107"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="B108:B109"/>
-    <mergeCell ref="A110:A111"/>
-    <mergeCell ref="B110:B111"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="B112:B113"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="B116:B117"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="B120:B121"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="A124:A125"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="B126:B127"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="B128:B129"/>
-    <mergeCell ref="A140:A141"/>
-    <mergeCell ref="B140:B141"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:B143"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="B134:B135"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="B138:B139"/>
-    <mergeCell ref="GH11:GJ11"/>
-    <mergeCell ref="GK11:GM11"/>
-    <mergeCell ref="GN11:GP11"/>
-    <mergeCell ref="GQ11:GS11"/>
-    <mergeCell ref="GT11:GV11"/>
-    <mergeCell ref="GW11:GY11"/>
-    <mergeCell ref="GZ11:HB11"/>
-    <mergeCell ref="HC11:HE11"/>
-    <mergeCell ref="HF11:HH11"/>
-    <mergeCell ref="HI11:HK11"/>
-    <mergeCell ref="HL11:HN11"/>
-    <mergeCell ref="HO11:HQ11"/>
-    <mergeCell ref="HR11:HT11"/>
-    <mergeCell ref="HU11:HW11"/>
-    <mergeCell ref="HX11:HZ11"/>
-    <mergeCell ref="IA11:IC11"/>
-    <mergeCell ref="ID11:IF11"/>
-    <mergeCell ref="IG11:II11"/>
-    <mergeCell ref="JK11:JM11"/>
-    <mergeCell ref="JN11:JP11"/>
-    <mergeCell ref="JQ11:JS11"/>
-    <mergeCell ref="JT11:JV11"/>
-    <mergeCell ref="JW11:JY11"/>
-    <mergeCell ref="JZ11:KB11"/>
-    <mergeCell ref="KC11:KE11"/>
-    <mergeCell ref="IJ11:IL11"/>
-    <mergeCell ref="IM11:IO11"/>
-    <mergeCell ref="IP11:IR11"/>
-    <mergeCell ref="IS11:IU11"/>
-    <mergeCell ref="IV11:IX11"/>
-    <mergeCell ref="IY11:JA11"/>
-    <mergeCell ref="JB11:JD11"/>
-    <mergeCell ref="JE11:JG11"/>
-    <mergeCell ref="JH11:JJ11"/>
   </mergeCells>
   <conditionalFormatting sqref="D14:F14">
     <cfRule type="expression" dxfId="699" priority="892">

</xml_diff>